<commit_message>
Craigslist raw and aggregate data update
Also updated project prototype excel sheet and AggregateData.py file.
</commit_message>
<xml_diff>
--- a/AggregateCraigslistData.xlsx
+++ b/AggregateCraigslistData.xlsx
@@ -750,16 +750,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>2.058823529411764</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>1010.473684210526</v>
+        <v>1019.045454545455</v>
       </c>
       <c r="D2">
-        <v>1005.5</v>
+        <v>998.8181818181819</v>
       </c>
       <c r="E2">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -767,16 +767,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>1.962962962962963</v>
+        <v>2.107142857142857</v>
       </c>
       <c r="C3">
-        <v>738.1428571428571</v>
+        <v>730.9722222222222</v>
       </c>
       <c r="D3">
         <v>1335</v>
       </c>
       <c r="E3">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -832,10 +832,10 @@
         <v>1.558333333333333</v>
       </c>
       <c r="C7">
-        <v>967.7166666666667</v>
+        <v>963.5916666666667</v>
       </c>
       <c r="D7">
-        <v>982.6567164179105</v>
+        <v>980.8059701492538</v>
       </c>
       <c r="E7">
         <v>120</v>
@@ -846,16 +846,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>2.194444444444445</v>
+        <v>2.138888888888889</v>
       </c>
       <c r="C8">
-        <v>670.560975609756</v>
+        <v>670.6666666666666</v>
       </c>
       <c r="D8">
-        <v>889.7777777777778</v>
+        <v>874.1</v>
       </c>
       <c r="E8">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -863,16 +863,16 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>2.357142857142857</v>
+        <v>2.3125</v>
       </c>
       <c r="C9">
-        <v>742.5</v>
+        <v>762.1052631578947</v>
       </c>
       <c r="D9">
-        <v>1145</v>
+        <v>1163.333333333333</v>
       </c>
       <c r="E9">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -897,16 +897,16 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>1.9375</v>
+        <v>1.866666666666667</v>
       </c>
       <c r="C11">
-        <v>1010.3125</v>
+        <v>945.6666666666666</v>
       </c>
       <c r="D11">
-        <v>1210</v>
+        <v>1278.333333333333</v>
       </c>
       <c r="E11">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -936,13 +936,13 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>2.461538461538462</v>
+        <v>2.485981308411215</v>
       </c>
       <c r="C14">
-        <v>645.1052631578947</v>
+        <v>629.7913043478261</v>
       </c>
       <c r="D14">
-        <v>1211.842105263158</v>
+        <v>1138.764705882353</v>
       </c>
       <c r="E14">
         <v>120</v>
@@ -970,16 +970,16 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>2.068181818181818</v>
+        <v>2.066666666666667</v>
       </c>
       <c r="C16">
-        <v>734.64</v>
+        <v>740.8235294117648</v>
       </c>
       <c r="D16">
-        <v>920.5384615384615</v>
+        <v>917.8</v>
       </c>
       <c r="E16">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1004,13 +1004,13 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>1.571428571428571</v>
+        <v>1.558558558558559</v>
       </c>
       <c r="C18">
-        <v>823.6134453781513</v>
+        <v>821.09243697479</v>
       </c>
       <c r="D18">
-        <v>822</v>
+        <v>811.5599999999999</v>
       </c>
       <c r="E18">
         <v>120</v>
@@ -1021,16 +1021,16 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>2.194444444444445</v>
+        <v>2.137931034482758</v>
       </c>
       <c r="C19">
-        <v>954.1282051282051</v>
+        <v>955.25</v>
       </c>
       <c r="D19">
-        <v>1448.9</v>
+        <v>1322.75</v>
       </c>
       <c r="E19">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1038,16 +1038,16 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>1.666666666666667</v>
+        <v>1.571428571428571</v>
       </c>
       <c r="C20">
-        <v>557.3333333333334</v>
+        <v>525.7142857142857</v>
       </c>
       <c r="D20">
         <v>700</v>
       </c>
       <c r="E20">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1058,13 +1058,13 @@
         <v>2.571428571428572</v>
       </c>
       <c r="C21">
-        <v>1158.125</v>
+        <v>1181.428571428571</v>
       </c>
       <c r="D21">
         <v>1474.4</v>
       </c>
       <c r="E21">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1089,16 +1089,16 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>2.583333333333333</v>
+        <v>2.7</v>
       </c>
       <c r="C23">
-        <v>895.3846153846154</v>
+        <v>885.4545454545455</v>
       </c>
       <c r="D23">
-        <v>1059.5</v>
+        <v>1063.333333333333</v>
       </c>
       <c r="E23">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1106,16 +1106,16 @@
         <v>26</v>
       </c>
       <c r="B24">
-        <v>1.722222222222222</v>
+        <v>1.823529411764706</v>
       </c>
       <c r="C24">
-        <v>505.3181818181818</v>
+        <v>508.4285714285714</v>
       </c>
       <c r="D24">
         <v>925</v>
       </c>
       <c r="E24">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1123,16 +1123,16 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>1.607142857142857</v>
+        <v>1.52054794520548</v>
       </c>
       <c r="C25">
-        <v>639.8666666666667</v>
+        <v>624.7012987012987</v>
       </c>
       <c r="D25">
-        <v>695.1923076923077</v>
+        <v>691.40625</v>
       </c>
       <c r="E25">
-        <v>60</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1140,16 +1140,16 @@
         <v>28</v>
       </c>
       <c r="B26">
-        <v>1.893617021276596</v>
+        <v>1.895833333333333</v>
       </c>
       <c r="C26">
-        <v>738.8571428571429</v>
+        <v>741.58</v>
       </c>
       <c r="D26">
-        <v>897.25</v>
+        <v>941</v>
       </c>
       <c r="E26">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1157,16 +1157,16 @@
         <v>29</v>
       </c>
       <c r="B27">
-        <v>2.142857142857143</v>
+        <v>2.166666666666667</v>
       </c>
       <c r="C27">
-        <v>584.5</v>
+        <v>572.2222222222222</v>
       </c>
       <c r="D27">
         <v>1050</v>
       </c>
       <c r="E27">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1191,7 +1191,7 @@
         <v>2.1</v>
       </c>
       <c r="C29">
-        <v>1050.454545454545</v>
+        <v>1043.636363636364</v>
       </c>
       <c r="D29">
         <v>1098</v>
@@ -1205,16 +1205,16 @@
         <v>32</v>
       </c>
       <c r="B30">
-        <v>2.1875</v>
+        <v>2.133333333333333</v>
       </c>
       <c r="C30">
-        <v>668.2352941176471</v>
+        <v>663.125</v>
       </c>
       <c r="D30">
         <v>1125</v>
       </c>
       <c r="E30">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1222,16 +1222,16 @@
         <v>33</v>
       </c>
       <c r="B31">
-        <v>1.6</v>
+        <v>1.652173913043478</v>
       </c>
       <c r="C31">
-        <v>799.074074074074</v>
+        <v>810</v>
       </c>
       <c r="D31">
-        <v>912.7857142857143</v>
+        <v>931.5833333333334</v>
       </c>
       <c r="E31">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1273,16 +1273,16 @@
         <v>36</v>
       </c>
       <c r="B34">
-        <v>2.261904761904762</v>
+        <v>2.285714285714286</v>
       </c>
       <c r="C34">
-        <v>821.063829787234</v>
+        <v>821.195652173913</v>
       </c>
       <c r="D34">
-        <v>1270.181818181818</v>
+        <v>1271.2</v>
       </c>
       <c r="E34">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1290,10 +1290,10 @@
         <v>37</v>
       </c>
       <c r="B35">
-        <v>2.1</v>
+        <v>2.2</v>
       </c>
       <c r="C35">
-        <v>846</v>
+        <v>866.5</v>
       </c>
       <c r="D35">
         <v>1330.25</v>
@@ -1321,16 +1321,16 @@
         <v>39</v>
       </c>
       <c r="B37">
-        <v>1.640625</v>
+        <v>1.661290322580645</v>
       </c>
       <c r="C37">
-        <v>611.7042253521126</v>
+        <v>610.2285714285714</v>
       </c>
       <c r="D37">
-        <v>804.4042553191489</v>
+        <v>809.1590909090909</v>
       </c>
       <c r="E37">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1358,13 +1358,13 @@
         <v>2.111111111111111</v>
       </c>
       <c r="C39">
-        <v>1256.111111111111</v>
+        <v>1350.5</v>
       </c>
       <c r="D39">
         <v>1766.666666666667</v>
       </c>
       <c r="E39">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1372,16 +1372,16 @@
         <v>42</v>
       </c>
       <c r="B40">
-        <v>2.333333333333333</v>
+        <v>2.090909090909091</v>
       </c>
       <c r="C40">
-        <v>972.7777777777778</v>
+        <v>773.6363636363636</v>
       </c>
       <c r="D40">
-        <v>1266.666666666667</v>
+        <v>1000</v>
       </c>
       <c r="E40">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1389,16 +1389,16 @@
         <v>43</v>
       </c>
       <c r="B41">
-        <v>1.978723404255319</v>
+        <v>2.08695652173913</v>
       </c>
       <c r="C41">
-        <v>661.5666666666667</v>
+        <v>672.7413793103449</v>
       </c>
       <c r="D41">
-        <v>1253</v>
+        <v>1272.461538461539</v>
       </c>
       <c r="E41">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1406,16 +1406,16 @@
         <v>44</v>
       </c>
       <c r="B42">
-        <v>2.244444444444444</v>
+        <v>2.255813953488372</v>
       </c>
       <c r="C42">
-        <v>791.4772727272727</v>
+        <v>795.952380952381</v>
       </c>
       <c r="D42">
         <v>969.0434782608696</v>
       </c>
       <c r="E42">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1423,16 +1423,16 @@
         <v>45</v>
       </c>
       <c r="B43">
-        <v>1.821428571428571</v>
+        <v>1.855421686746988</v>
       </c>
       <c r="C43">
-        <v>671.1411764705882</v>
+        <v>675.0357142857143</v>
       </c>
       <c r="D43">
         <v>1014.848484848485</v>
       </c>
       <c r="E43">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1440,16 +1440,16 @@
         <v>46</v>
       </c>
       <c r="B44">
-        <v>2.2</v>
+        <v>2</v>
       </c>
       <c r="C44">
-        <v>832.5</v>
+        <v>723.3333333333334</v>
       </c>
       <c r="D44">
-        <v>1437</v>
+        <v>1200</v>
       </c>
       <c r="E44">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1474,16 +1474,16 @@
         <v>48</v>
       </c>
       <c r="B46">
-        <v>2.166666666666667</v>
+        <v>2.090909090909091</v>
       </c>
       <c r="C46">
-        <v>2681.538461538461</v>
+        <v>2855</v>
       </c>
       <c r="D46">
         <v>640</v>
       </c>
       <c r="E46">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1491,16 +1491,16 @@
         <v>49</v>
       </c>
       <c r="B47">
-        <v>2.0625</v>
+        <v>2.053191489361702</v>
       </c>
       <c r="C47">
-        <v>1063.422680412371</v>
+        <v>1073.136842105263</v>
       </c>
       <c r="D47">
-        <v>1050.537313432836</v>
+        <v>1048.867647058823</v>
       </c>
       <c r="E47">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1516,16 +1516,16 @@
         <v>51</v>
       </c>
       <c r="B49">
-        <v>2.571428571428572</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="C49">
-        <v>1168.444444444444</v>
+        <v>1220.75</v>
       </c>
       <c r="D49">
-        <v>1550</v>
+        <v>1637.5</v>
       </c>
       <c r="E49">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1533,16 +1533,16 @@
         <v>52</v>
       </c>
       <c r="B50">
-        <v>2.045454545454545</v>
+        <v>2.041666666666667</v>
       </c>
       <c r="C50">
-        <v>755</v>
+        <v>744.6</v>
       </c>
       <c r="D50">
-        <v>1111.666666666667</v>
+        <v>1127.5</v>
       </c>
       <c r="E50">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1550,16 +1550,16 @@
         <v>53</v>
       </c>
       <c r="B51">
-        <v>2.033898305084746</v>
+        <v>2.070175438596491</v>
       </c>
       <c r="C51">
-        <v>664.375</v>
+        <v>666.3461538461538</v>
       </c>
       <c r="D51">
         <v>1030</v>
       </c>
       <c r="E51">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1567,16 +1567,16 @@
         <v>54</v>
       </c>
       <c r="B52">
-        <v>1.533333333333333</v>
+        <v>1.602150537634409</v>
       </c>
       <c r="C52">
-        <v>632.7802197802198</v>
+        <v>645.6170212765958</v>
       </c>
       <c r="D52">
-        <v>733.5</v>
+        <v>800.8125</v>
       </c>
       <c r="E52">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1584,16 +1584,13 @@
         <v>55</v>
       </c>
       <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53">
+        <v>583.6666666666666</v>
+      </c>
+      <c r="E53">
         <v>3</v>
-      </c>
-      <c r="C53">
-        <v>625.25</v>
-      </c>
-      <c r="D53">
-        <v>450</v>
-      </c>
-      <c r="E53">
-        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1601,16 +1598,16 @@
         <v>56</v>
       </c>
       <c r="B54">
-        <v>1.870967741935484</v>
+        <v>1.866666666666667</v>
       </c>
       <c r="C54">
-        <v>1122.625</v>
+        <v>1146.633333333333</v>
       </c>
       <c r="D54">
         <v>1172.642857142857</v>
       </c>
       <c r="E54">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1618,16 +1615,16 @@
         <v>57</v>
       </c>
       <c r="B55">
-        <v>1.967741935483871</v>
+        <v>2.066666666666667</v>
       </c>
       <c r="C55">
-        <v>646.5135135135135</v>
+        <v>653.2222222222222</v>
       </c>
       <c r="D55">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="E55">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1635,13 +1632,13 @@
         <v>58</v>
       </c>
       <c r="B56">
-        <v>2.010869565217391</v>
+        <v>2.021739130434783</v>
       </c>
       <c r="C56">
-        <v>1141.975</v>
+        <v>1134.475</v>
       </c>
       <c r="D56">
-        <v>1299.354838709677</v>
+        <v>1240.2</v>
       </c>
       <c r="E56">
         <v>120</v>
@@ -1652,13 +1649,13 @@
         <v>59</v>
       </c>
       <c r="B57">
-        <v>1.864864864864865</v>
+        <v>1.854545454545454</v>
       </c>
       <c r="C57">
-        <v>806.0916666666667</v>
+        <v>804.4</v>
       </c>
       <c r="D57">
-        <v>1179.565217391304</v>
+        <v>1089.181818181818</v>
       </c>
       <c r="E57">
         <v>120</v>
@@ -1669,13 +1666,13 @@
         <v>60</v>
       </c>
       <c r="B58">
-        <v>1.920353982300885</v>
+        <v>1.911504424778761</v>
       </c>
       <c r="C58">
-        <v>1417.241666666667</v>
+        <v>1435.316666666667</v>
       </c>
       <c r="D58">
-        <v>1104.882352941177</v>
+        <v>1098.686567164179</v>
       </c>
       <c r="E58">
         <v>120</v>
@@ -1686,16 +1683,16 @@
         <v>61</v>
       </c>
       <c r="B59">
-        <v>2.372549019607843</v>
+        <v>2.416666666666667</v>
       </c>
       <c r="C59">
-        <v>804.5384615384615</v>
+        <v>809.9591836734694</v>
       </c>
       <c r="D59">
-        <v>1389.9</v>
+        <v>1322.111111111111</v>
       </c>
       <c r="E59">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1703,13 +1700,13 @@
         <v>62</v>
       </c>
       <c r="B60">
-        <v>1.973214285714286</v>
+        <v>1.982142857142857</v>
       </c>
       <c r="C60">
-        <v>1274.453781512605</v>
+        <v>1290.924369747899</v>
       </c>
       <c r="D60">
-        <v>964.25</v>
+        <v>952.3529411764706</v>
       </c>
       <c r="E60">
         <v>120</v>
@@ -1720,13 +1717,13 @@
         <v>63</v>
       </c>
       <c r="B61">
-        <v>1.8125</v>
+        <v>1.956521739130435</v>
       </c>
       <c r="C61">
-        <v>1121.302521008403</v>
+        <v>1133.058333333333</v>
       </c>
       <c r="D61">
-        <v>984.1</v>
+        <v>1059.375</v>
       </c>
       <c r="E61">
         <v>120</v>
@@ -1737,16 +1734,16 @@
         <v>64</v>
       </c>
       <c r="B62">
-        <v>2.122448979591837</v>
+        <v>2.125</v>
       </c>
       <c r="C62">
-        <v>880.9830508474577</v>
+        <v>887.3684210526316</v>
       </c>
       <c r="D62">
-        <v>1250.8125</v>
+        <v>1275.533333333333</v>
       </c>
       <c r="E62">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1754,13 +1751,13 @@
         <v>65</v>
       </c>
       <c r="B63">
-        <v>1.897435897435897</v>
+        <v>1.956521739130435</v>
       </c>
       <c r="C63">
-        <v>1075.083333333333</v>
+        <v>1086.975</v>
       </c>
       <c r="D63">
-        <v>1309.214285714286</v>
+        <v>1411.530612244898</v>
       </c>
       <c r="E63">
         <v>120</v>
@@ -1771,13 +1768,13 @@
         <v>66</v>
       </c>
       <c r="B64">
-        <v>1.743362831858407</v>
+        <v>1.725663716814159</v>
       </c>
       <c r="C64">
-        <v>847.075</v>
+        <v>850.9416666666667</v>
       </c>
       <c r="D64">
-        <v>758.0555555555555</v>
+        <v>756.697247706422</v>
       </c>
       <c r="E64">
         <v>120</v>
@@ -1788,13 +1785,13 @@
         <v>67</v>
       </c>
       <c r="B65">
-        <v>2.541284403669725</v>
+        <v>2.532110091743119</v>
       </c>
       <c r="C65">
-        <v>944.9495798319327</v>
+        <v>940.7563025210084</v>
       </c>
       <c r="D65">
-        <v>1170</v>
+        <v>1192.066666666667</v>
       </c>
       <c r="E65">
         <v>120</v>
@@ -1805,13 +1802,13 @@
         <v>68</v>
       </c>
       <c r="B66">
-        <v>2.15929203539823</v>
+        <v>2.194690265486726</v>
       </c>
       <c r="C66">
-        <v>1035.241666666667</v>
+        <v>1023.491666666667</v>
       </c>
       <c r="D66">
-        <v>1362.511627906977</v>
+        <v>1355.782608695652</v>
       </c>
       <c r="E66">
         <v>120</v>
@@ -1822,13 +1819,13 @@
         <v>69</v>
       </c>
       <c r="B67">
-        <v>2.247524752475248</v>
+        <v>2.180851063829787</v>
       </c>
       <c r="C67">
-        <v>1036.75</v>
+        <v>1062.141666666667</v>
       </c>
       <c r="D67">
-        <v>932.0941176470589</v>
+        <v>914.934065934066</v>
       </c>
       <c r="E67">
         <v>120</v>
@@ -1839,13 +1836,13 @@
         <v>70</v>
       </c>
       <c r="B68">
-        <v>2.924731182795699</v>
+        <v>2.915789473684211</v>
       </c>
       <c r="C68">
-        <v>1646.016666666667</v>
+        <v>1532.283333333333</v>
       </c>
       <c r="D68">
-        <v>1148.363636363636</v>
+        <v>1306.571428571429</v>
       </c>
       <c r="E68">
         <v>120</v>
@@ -1856,16 +1853,16 @@
         <v>71</v>
       </c>
       <c r="B69">
-        <v>2.353448275862069</v>
+        <v>2.339285714285714</v>
       </c>
       <c r="C69">
-        <v>1026.991525423729</v>
+        <v>1025.852173913044</v>
       </c>
       <c r="D69">
-        <v>1187.72</v>
+        <v>1184.666666666667</v>
       </c>
       <c r="E69">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1873,16 +1870,16 @@
         <v>72</v>
       </c>
       <c r="B70">
-        <v>2.054794520547945</v>
+        <v>2.067567567567568</v>
       </c>
       <c r="C70">
-        <v>1041.578947368421</v>
+        <v>1035.320512820513</v>
       </c>
       <c r="D70">
-        <v>1184.758620689655</v>
+        <v>1185.266666666667</v>
       </c>
       <c r="E70">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -1890,13 +1887,13 @@
         <v>73</v>
       </c>
       <c r="B71">
-        <v>1.888888888888889</v>
+        <v>1.906542056074766</v>
       </c>
       <c r="C71">
-        <v>937.90756302521</v>
+        <v>938.2016806722689</v>
       </c>
       <c r="D71">
-        <v>1180.029411764706</v>
+        <v>1174.483870967742</v>
       </c>
       <c r="E71">
         <v>120</v>
@@ -1907,13 +1904,13 @@
         <v>74</v>
       </c>
       <c r="B72">
-        <v>1.646017699115044</v>
+        <v>1.464285714285714</v>
       </c>
       <c r="C72">
-        <v>1218.175</v>
+        <v>1106.75</v>
       </c>
       <c r="D72">
-        <v>896.2205882352941</v>
+        <v>813.0547945205479</v>
       </c>
       <c r="E72">
         <v>120</v>
@@ -1924,13 +1921,13 @@
         <v>75</v>
       </c>
       <c r="B73">
-        <v>1.596330275229358</v>
+        <v>1.577981651376147</v>
       </c>
       <c r="C73">
-        <v>865.975</v>
+        <v>869.4083333333333</v>
       </c>
       <c r="D73">
-        <v>781.8780487804878</v>
+        <v>787.0714285714286</v>
       </c>
       <c r="E73">
         <v>120</v>
@@ -1941,13 +1938,13 @@
         <v>76</v>
       </c>
       <c r="B74">
-        <v>1.821782178217822</v>
+        <v>1.85</v>
       </c>
       <c r="C74">
-        <v>1507.126050420168</v>
+        <v>1519.453781512605</v>
       </c>
       <c r="D74">
-        <v>1149.309278350516</v>
+        <v>1152.053191489362</v>
       </c>
       <c r="E74">
         <v>120</v>
@@ -1958,16 +1955,16 @@
         <v>77</v>
       </c>
       <c r="B75">
-        <v>2.210526315789474</v>
+        <v>2.222222222222222</v>
       </c>
       <c r="C75">
-        <v>1068.947368421053</v>
+        <v>1083.888888888889</v>
       </c>
       <c r="D75">
-        <v>1377.277777777778</v>
+        <v>1371.722222222222</v>
       </c>
       <c r="E75">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1975,13 +1972,13 @@
         <v>78</v>
       </c>
       <c r="B76">
-        <v>1.785714285714286</v>
+        <v>1.823008849557522</v>
       </c>
       <c r="C76">
-        <v>1003.672268907563</v>
+        <v>1005.941176470588</v>
       </c>
       <c r="D76">
-        <v>1156.673076923077</v>
+        <v>1183.738461538461</v>
       </c>
       <c r="E76">
         <v>120</v>
@@ -1992,13 +1989,13 @@
         <v>79</v>
       </c>
       <c r="B77">
-        <v>1.552380952380952</v>
+        <v>1.485436893203884</v>
       </c>
       <c r="C77">
-        <v>1511.125</v>
+        <v>1437.766666666667</v>
       </c>
       <c r="D77">
-        <v>860.0886075949367</v>
+        <v>804.5714285714286</v>
       </c>
       <c r="E77">
         <v>120</v>
@@ -2009,16 +2006,16 @@
         <v>80</v>
       </c>
       <c r="B78">
-        <v>2.076923076923077</v>
+        <v>1.875</v>
       </c>
       <c r="C78">
-        <v>816.1153846153846</v>
+        <v>781.625</v>
       </c>
       <c r="D78">
-        <v>1115</v>
+        <v>1124</v>
       </c>
       <c r="E78">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -2026,13 +2023,13 @@
         <v>81</v>
       </c>
       <c r="B79">
-        <v>2.235849056603774</v>
+        <v>2.287037037037037</v>
       </c>
       <c r="C79">
-        <v>1325.291666666667</v>
+        <v>1355.883333333333</v>
       </c>
       <c r="D79">
-        <v>788.6666666666666</v>
+        <v>889.4571428571429</v>
       </c>
       <c r="E79">
         <v>120</v>
@@ -2060,13 +2057,13 @@
         <v>83</v>
       </c>
       <c r="B81">
-        <v>1.875</v>
+        <v>1.900900900900901</v>
       </c>
       <c r="C81">
-        <v>1257.512605042017</v>
+        <v>1250.915966386555</v>
       </c>
       <c r="D81">
-        <v>1462.086956521739</v>
+        <v>1429.846153846154</v>
       </c>
       <c r="E81">
         <v>120</v>
@@ -2077,16 +2074,16 @@
         <v>84</v>
       </c>
       <c r="B82">
-        <v>1.813333333333333</v>
+        <v>1.794520547945206</v>
       </c>
       <c r="C82">
-        <v>786.0875</v>
+        <v>793.1558441558442</v>
       </c>
       <c r="D82">
-        <v>939.8611111111111</v>
+        <v>930.0555555555555</v>
       </c>
       <c r="E82">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -2094,13 +2091,13 @@
         <v>85</v>
       </c>
       <c r="B83">
-        <v>1.695652173913043</v>
+        <v>1.747826086956522</v>
       </c>
       <c r="C83">
-        <v>1105.35</v>
+        <v>1079.458333333333</v>
       </c>
       <c r="D83">
-        <v>902.8125</v>
+        <v>924.3166666666667</v>
       </c>
       <c r="E83">
         <v>120</v>
@@ -2111,16 +2108,16 @@
         <v>86</v>
       </c>
       <c r="B84">
-        <v>1.584615384615385</v>
+        <v>1.59375</v>
       </c>
       <c r="C84">
-        <v>1042.95652173913</v>
+        <v>1047.279411764706</v>
       </c>
       <c r="D84">
         <v>1351.222222222222</v>
       </c>
       <c r="E84">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -2128,13 +2125,13 @@
         <v>87</v>
       </c>
       <c r="B85">
-        <v>1.63963963963964</v>
+        <v>1.558558558558559</v>
       </c>
       <c r="C85">
-        <v>1404.275</v>
+        <v>1401.083333333333</v>
       </c>
       <c r="D85">
-        <v>997.975</v>
+        <v>967.8928571428571</v>
       </c>
       <c r="E85">
         <v>120</v>
@@ -2145,16 +2142,16 @@
         <v>88</v>
       </c>
       <c r="B86">
-        <v>1.655172413793103</v>
+        <v>1.662921348314607</v>
       </c>
       <c r="C86">
-        <v>905.659793814433</v>
+        <v>907.9191919191919</v>
       </c>
       <c r="D86">
-        <v>1151.974358974359</v>
+        <v>1151.925</v>
       </c>
       <c r="E86">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -2162,16 +2159,16 @@
         <v>89</v>
       </c>
       <c r="B87">
-        <v>2.11864406779661</v>
+        <v>2.063492063492064</v>
       </c>
       <c r="C87">
-        <v>926.8648648648649</v>
+        <v>913.8947368421053</v>
       </c>
       <c r="D87">
         <v>1222.5</v>
       </c>
       <c r="E87">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -2179,16 +2176,16 @@
         <v>90</v>
       </c>
       <c r="B88">
-        <v>2.087719298245614</v>
+        <v>2.070175438596491</v>
       </c>
       <c r="C88">
-        <v>808.344262295082</v>
+        <v>817.1967213114754</v>
       </c>
       <c r="D88">
-        <v>999.8888888888889</v>
+        <v>1029.294117647059</v>
       </c>
       <c r="E88">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -2196,16 +2193,16 @@
         <v>91</v>
       </c>
       <c r="B89">
-        <v>1.595744680851064</v>
+        <v>1.58695652173913</v>
       </c>
       <c r="C89">
-        <v>822.96875</v>
+        <v>822.2786885245902</v>
       </c>
       <c r="D89">
-        <v>1065</v>
+        <v>1077.368421052632</v>
       </c>
       <c r="E89">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -2213,13 +2210,13 @@
         <v>92</v>
       </c>
       <c r="B90">
-        <v>1.456140350877193</v>
+        <v>1.447368421052632</v>
       </c>
       <c r="C90">
-        <v>970.3166666666667</v>
+        <v>961.4333333333333</v>
       </c>
       <c r="D90">
-        <v>856.1898734177215</v>
+        <v>830.4197530864197</v>
       </c>
       <c r="E90">
         <v>120</v>
@@ -2230,16 +2227,16 @@
         <v>93</v>
       </c>
       <c r="B91">
-        <v>3.146341463414634</v>
+        <v>3.108695652173913</v>
       </c>
       <c r="C91">
-        <v>2221.627906976744</v>
+        <v>2151.666666666667</v>
       </c>
       <c r="D91">
-        <v>2089.857142857143</v>
+        <v>1899.64705882353</v>
       </c>
       <c r="E91">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -2247,16 +2244,16 @@
         <v>94</v>
       </c>
       <c r="B92">
-        <v>2.315789473684211</v>
+        <v>2.277777777777778</v>
       </c>
       <c r="C92">
-        <v>875.95</v>
+        <v>895.7894736842105</v>
       </c>
       <c r="D92">
         <v>1682.5</v>
       </c>
       <c r="E92">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -2267,10 +2264,10 @@
         <v>1.466666666666667</v>
       </c>
       <c r="C93">
-        <v>1251.333333333333</v>
+        <v>1245.583333333333</v>
       </c>
       <c r="D93">
-        <v>871.9217391304347</v>
+        <v>870.0521739130435</v>
       </c>
       <c r="E93">
         <v>120</v>
@@ -2281,16 +2278,16 @@
         <v>96</v>
       </c>
       <c r="B94">
-        <v>2.111111111111111</v>
+        <v>2.176470588235294</v>
       </c>
       <c r="C94">
-        <v>1188.75</v>
+        <v>1206.578947368421</v>
       </c>
       <c r="D94">
-        <v>1742.555555555556</v>
+        <v>1860.375</v>
       </c>
       <c r="E94">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -2298,13 +2295,13 @@
         <v>97</v>
       </c>
       <c r="B95">
-        <v>3.147826086956522</v>
+        <v>3.191304347826087</v>
       </c>
       <c r="C95">
-        <v>1797.683333333333</v>
+        <v>1805.108333333333</v>
       </c>
       <c r="D95">
-        <v>1148.277777777778</v>
+        <v>1341.380952380952</v>
       </c>
       <c r="E95">
         <v>120</v>
@@ -2394,16 +2391,16 @@
         <v>103</v>
       </c>
       <c r="B101">
-        <v>1.925925925925926</v>
+        <v>1.961538461538461</v>
       </c>
       <c r="C101">
-        <v>1245.166666666667</v>
+        <v>1264.827586206897</v>
       </c>
       <c r="D101">
         <v>1244.133333333333</v>
       </c>
       <c r="E101">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -2411,16 +2408,16 @@
         <v>104</v>
       </c>
       <c r="B102">
-        <v>1.210526315789474</v>
+        <v>1.23728813559322</v>
       </c>
       <c r="C102">
-        <v>747.6666666666666</v>
+        <v>756.5333333333333</v>
       </c>
       <c r="D102">
-        <v>788.8333333333334</v>
+        <v>784</v>
       </c>
       <c r="E102">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -2428,16 +2425,16 @@
         <v>105</v>
       </c>
       <c r="B103">
-        <v>1.666666666666667</v>
+        <v>1.714285714285714</v>
       </c>
       <c r="C103">
-        <v>730.8333333333334</v>
+        <v>735</v>
       </c>
       <c r="D103">
         <v>1377</v>
       </c>
       <c r="E103">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -2448,7 +2445,7 @@
         <v>2.333333333333333</v>
       </c>
       <c r="C104">
-        <v>1212.5</v>
+        <v>1187.5</v>
       </c>
       <c r="E104">
         <v>4</v>
@@ -2459,16 +2456,16 @@
         <v>107</v>
       </c>
       <c r="B105">
-        <v>2</v>
+        <v>2.04</v>
       </c>
       <c r="C105">
-        <v>670.15625</v>
+        <v>675.6060606060606</v>
       </c>
       <c r="D105">
         <v>883.3333333333334</v>
       </c>
       <c r="E105">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2524,16 +2521,16 @@
         <v>111</v>
       </c>
       <c r="B109">
-        <v>1.810810810810811</v>
+        <v>1.82051282051282</v>
       </c>
       <c r="C109">
-        <v>800.0263157894736</v>
+        <v>795.275</v>
       </c>
       <c r="D109">
         <v>895.3</v>
       </c>
       <c r="E109">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -2541,16 +2538,16 @@
         <v>112</v>
       </c>
       <c r="B110">
-        <v>1.685714285714286</v>
+        <v>1.764705882352941</v>
       </c>
       <c r="C110">
-        <v>1489.166666666667</v>
+        <v>1508.857142857143</v>
       </c>
       <c r="D110">
-        <v>979.0333333333333</v>
+        <v>991.2857142857143</v>
       </c>
       <c r="E110">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -2558,16 +2555,16 @@
         <v>113</v>
       </c>
       <c r="B111">
-        <v>2.214285714285714</v>
+        <v>2.230769230769231</v>
       </c>
       <c r="C111">
-        <v>757.6</v>
+        <v>762.0714285714286</v>
       </c>
       <c r="D111">
         <v>1000</v>
       </c>
       <c r="E111">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -2575,16 +2572,16 @@
         <v>114</v>
       </c>
       <c r="B112">
-        <v>2.14</v>
+        <v>2.204081632653061</v>
       </c>
       <c r="C112">
-        <v>782.9622641509434</v>
+        <v>785.6923076923077</v>
       </c>
       <c r="D112">
-        <v>973.3333333333334</v>
+        <v>967.2</v>
       </c>
       <c r="E112">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -2606,13 +2603,13 @@
         <v>116</v>
       </c>
       <c r="B114">
-        <v>2.042553191489362</v>
+        <v>2.063829787234043</v>
       </c>
       <c r="C114">
-        <v>1578.36</v>
+        <v>1597.88</v>
       </c>
       <c r="D114">
-        <v>1044.513513513514</v>
+        <v>1049.194444444444</v>
       </c>
       <c r="E114">
         <v>50</v>
@@ -2623,16 +2620,16 @@
         <v>117</v>
       </c>
       <c r="B115">
-        <v>2.428571428571428</v>
+        <v>2.5</v>
       </c>
       <c r="C115">
-        <v>801.1111111111111</v>
+        <v>786</v>
       </c>
       <c r="D115">
         <v>1000</v>
       </c>
       <c r="E115">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated aggregatingFile and zillowData
</commit_message>
<xml_diff>
--- a/AggregateCraigslistData.xlsx
+++ b/AggregateCraigslistData.xlsx
@@ -767,16 +767,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>2.107142857142857</v>
+        <v>2.137931034482758</v>
       </c>
       <c r="C3">
-        <v>730.9722222222222</v>
+        <v>727.4324324324324</v>
       </c>
       <c r="D3">
         <v>1335</v>
       </c>
       <c r="E3">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -829,13 +829,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>1.558333333333333</v>
+        <v>1.541666666666667</v>
       </c>
       <c r="C7">
-        <v>963.5916666666667</v>
+        <v>958.8</v>
       </c>
       <c r="D7">
-        <v>980.8059701492538</v>
+        <v>974.1176470588235</v>
       </c>
       <c r="E7">
         <v>120</v>
@@ -863,16 +863,16 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>2.3125</v>
+        <v>2.375</v>
       </c>
       <c r="C9">
-        <v>762.1052631578947</v>
+        <v>755.5555555555555</v>
       </c>
       <c r="D9">
-        <v>1163.333333333333</v>
+        <v>1140</v>
       </c>
       <c r="E9">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -897,16 +897,16 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>1.866666666666667</v>
+        <v>1.875</v>
       </c>
       <c r="C11">
-        <v>945.6666666666666</v>
+        <v>936.25</v>
       </c>
       <c r="D11">
         <v>1278.333333333333</v>
       </c>
       <c r="E11">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -936,13 +936,13 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>2.485981308411215</v>
+        <v>2.537735849056604</v>
       </c>
       <c r="C14">
-        <v>629.7913043478261</v>
+        <v>652.9912280701755</v>
       </c>
       <c r="D14">
-        <v>1138.764705882353</v>
+        <v>1113.941176470588</v>
       </c>
       <c r="E14">
         <v>120</v>
@@ -953,16 +953,16 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>2.222222222222222</v>
+        <v>2.285714285714286</v>
       </c>
       <c r="C15">
-        <v>833.3333333333334</v>
+        <v>842.8571428571429</v>
       </c>
       <c r="D15">
         <v>1625</v>
       </c>
       <c r="E15">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -973,7 +973,7 @@
         <v>2.066666666666667</v>
       </c>
       <c r="C16">
-        <v>740.8235294117648</v>
+        <v>739.843137254902</v>
       </c>
       <c r="D16">
         <v>917.8</v>
@@ -987,16 +987,16 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>2.333333333333333</v>
+        <v>3</v>
       </c>
       <c r="C17">
-        <v>983.3333333333334</v>
+        <v>1437.5</v>
       </c>
       <c r="D17">
         <v>1500</v>
       </c>
       <c r="E17">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1004,13 +1004,13 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>1.558558558558559</v>
+        <v>1.536363636363636</v>
       </c>
       <c r="C18">
-        <v>821.09243697479</v>
+        <v>819.1949152542373</v>
       </c>
       <c r="D18">
-        <v>811.5599999999999</v>
+        <v>827.4150943396227</v>
       </c>
       <c r="E18">
         <v>120</v>
@@ -1021,16 +1021,16 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>2.137931034482758</v>
+        <v>2.107142857142857</v>
       </c>
       <c r="C19">
-        <v>955.25</v>
+        <v>947.3548387096774</v>
       </c>
       <c r="D19">
         <v>1322.75</v>
       </c>
       <c r="E19">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1038,16 +1038,16 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>1.571428571428571</v>
+        <v>1.538461538461539</v>
       </c>
       <c r="C20">
-        <v>525.7142857142857</v>
+        <v>520</v>
       </c>
       <c r="D20">
         <v>700</v>
       </c>
       <c r="E20">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1055,16 +1055,16 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>2.571428571428572</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="C21">
-        <v>1181.428571428571</v>
+        <v>1203.333333333333</v>
       </c>
       <c r="D21">
         <v>1474.4</v>
       </c>
       <c r="E21">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1089,16 +1089,16 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>2.7</v>
+        <v>2.777777777777778</v>
       </c>
       <c r="C23">
-        <v>885.4545454545455</v>
+        <v>909</v>
       </c>
       <c r="D23">
         <v>1063.333333333333</v>
       </c>
       <c r="E23">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1109,13 +1109,13 @@
         <v>1.823529411764706</v>
       </c>
       <c r="C24">
-        <v>508.4285714285714</v>
+        <v>514.1</v>
       </c>
       <c r="D24">
         <v>925</v>
       </c>
       <c r="E24">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1123,16 +1123,16 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>1.52054794520548</v>
+        <v>1.5</v>
       </c>
       <c r="C25">
-        <v>624.7012987012987</v>
+        <v>622</v>
       </c>
       <c r="D25">
         <v>691.40625</v>
       </c>
       <c r="E25">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1140,16 +1140,16 @@
         <v>28</v>
       </c>
       <c r="B26">
-        <v>1.895833333333333</v>
+        <v>1.911111111111111</v>
       </c>
       <c r="C26">
-        <v>741.58</v>
+        <v>740.936170212766</v>
       </c>
       <c r="D26">
-        <v>941</v>
+        <v>979.6666666666666</v>
       </c>
       <c r="E26">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1208,7 +1208,7 @@
         <v>2.133333333333333</v>
       </c>
       <c r="C30">
-        <v>663.125</v>
+        <v>660</v>
       </c>
       <c r="D30">
         <v>1125</v>
@@ -1222,16 +1222,16 @@
         <v>33</v>
       </c>
       <c r="B31">
-        <v>1.652173913043478</v>
+        <v>1.9375</v>
       </c>
       <c r="C31">
-        <v>810</v>
+        <v>870</v>
       </c>
       <c r="D31">
-        <v>931.5833333333334</v>
+        <v>1025.571428571429</v>
       </c>
       <c r="E31">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1273,16 +1273,16 @@
         <v>36</v>
       </c>
       <c r="B34">
-        <v>2.285714285714286</v>
+        <v>2.3</v>
       </c>
       <c r="C34">
-        <v>821.195652173913</v>
+        <v>824.5454545454545</v>
       </c>
       <c r="D34">
-        <v>1271.2</v>
+        <v>1269.473684210526</v>
       </c>
       <c r="E34">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1290,16 +1290,16 @@
         <v>37</v>
       </c>
       <c r="B35">
-        <v>2.2</v>
+        <v>2.090909090909091</v>
       </c>
       <c r="C35">
-        <v>866.5</v>
+        <v>842.2727272727273</v>
       </c>
       <c r="D35">
-        <v>1330.25</v>
+        <v>1184.2</v>
       </c>
       <c r="E35">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1321,16 +1321,16 @@
         <v>39</v>
       </c>
       <c r="B37">
-        <v>1.661290322580645</v>
+        <v>1.639344262295082</v>
       </c>
       <c r="C37">
-        <v>610.2285714285714</v>
+        <v>610.8115942028985</v>
       </c>
       <c r="D37">
-        <v>809.1590909090909</v>
+        <v>810.6</v>
       </c>
       <c r="E37">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1338,13 +1338,13 @@
         <v>40</v>
       </c>
       <c r="B38">
-        <v>1.714285714285714</v>
+        <v>1.846153846153846</v>
       </c>
       <c r="C38">
-        <v>1099.0625</v>
+        <v>1027.1875</v>
       </c>
       <c r="D38">
-        <v>1032.857142857143</v>
+        <v>1005</v>
       </c>
       <c r="E38">
         <v>16</v>
@@ -1389,16 +1389,16 @@
         <v>43</v>
       </c>
       <c r="B41">
-        <v>2.08695652173913</v>
+        <v>2.065217391304348</v>
       </c>
       <c r="C41">
-        <v>672.7413793103449</v>
+        <v>667.8070175438596</v>
       </c>
       <c r="D41">
-        <v>1272.461538461539</v>
+        <v>1253</v>
       </c>
       <c r="E41">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1406,13 +1406,13 @@
         <v>44</v>
       </c>
       <c r="B42">
-        <v>2.255813953488372</v>
+        <v>2.279069767441861</v>
       </c>
       <c r="C42">
-        <v>795.952380952381</v>
+        <v>797.1190476190476</v>
       </c>
       <c r="D42">
-        <v>969.0434782608696</v>
+        <v>968.3181818181819</v>
       </c>
       <c r="E42">
         <v>43</v>
@@ -1423,16 +1423,16 @@
         <v>45</v>
       </c>
       <c r="B43">
-        <v>1.855421686746988</v>
+        <v>1.865853658536585</v>
       </c>
       <c r="C43">
-        <v>675.0357142857143</v>
+        <v>679.4939759036145</v>
       </c>
       <c r="D43">
-        <v>1014.848484848485</v>
+        <v>1015.806451612903</v>
       </c>
       <c r="E43">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1457,16 +1457,16 @@
         <v>47</v>
       </c>
       <c r="B45">
-        <v>1.8</v>
+        <v>1.846153846153846</v>
       </c>
       <c r="C45">
-        <v>718.4375</v>
+        <v>735</v>
       </c>
       <c r="D45">
-        <v>898</v>
+        <v>903.75</v>
       </c>
       <c r="E45">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1491,16 +1491,16 @@
         <v>49</v>
       </c>
       <c r="B47">
-        <v>2.053191489361702</v>
+        <v>2.051546391752577</v>
       </c>
       <c r="C47">
-        <v>1073.136842105263</v>
+        <v>1078.724489795918</v>
       </c>
       <c r="D47">
-        <v>1048.867647058823</v>
+        <v>1045.647887323944</v>
       </c>
       <c r="E47">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1519,13 +1519,13 @@
         <v>2.666666666666667</v>
       </c>
       <c r="C49">
-        <v>1220.75</v>
+        <v>1281.428571428571</v>
       </c>
       <c r="D49">
         <v>1637.5</v>
       </c>
       <c r="E49">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1533,10 +1533,10 @@
         <v>52</v>
       </c>
       <c r="B50">
-        <v>2.041666666666667</v>
+        <v>2</v>
       </c>
       <c r="C50">
-        <v>744.6</v>
+        <v>743.6</v>
       </c>
       <c r="D50">
         <v>1127.5</v>
@@ -1550,16 +1550,16 @@
         <v>53</v>
       </c>
       <c r="B51">
-        <v>2.070175438596491</v>
+        <v>2.072727272727273</v>
       </c>
       <c r="C51">
-        <v>666.3461538461538</v>
+        <v>668.0921052631579</v>
       </c>
       <c r="D51">
         <v>1030</v>
       </c>
       <c r="E51">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1567,16 +1567,16 @@
         <v>54</v>
       </c>
       <c r="B52">
-        <v>1.602150537634409</v>
+        <v>1.578947368421053</v>
       </c>
       <c r="C52">
-        <v>645.6170212765958</v>
+        <v>641.15625</v>
       </c>
       <c r="D52">
         <v>800.8125</v>
       </c>
       <c r="E52">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1584,13 +1584,13 @@
         <v>55</v>
       </c>
       <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>671.5</v>
+      </c>
+      <c r="E53">
         <v>4</v>
-      </c>
-      <c r="C53">
-        <v>583.6666666666666</v>
-      </c>
-      <c r="E53">
-        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1598,16 +1598,16 @@
         <v>56</v>
       </c>
       <c r="B54">
-        <v>1.866666666666667</v>
+        <v>1.903225806451613</v>
       </c>
       <c r="C54">
-        <v>1146.633333333333</v>
+        <v>1148.838709677419</v>
       </c>
       <c r="D54">
         <v>1172.642857142857</v>
       </c>
       <c r="E54">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1615,16 +1615,16 @@
         <v>57</v>
       </c>
       <c r="B55">
-        <v>2.066666666666667</v>
+        <v>2.064516129032258</v>
       </c>
       <c r="C55">
-        <v>653.2222222222222</v>
+        <v>653.1351351351351</v>
       </c>
       <c r="D55">
         <v>1100</v>
       </c>
       <c r="E55">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1632,13 +1632,13 @@
         <v>58</v>
       </c>
       <c r="B56">
-        <v>2.021739130434783</v>
+        <v>2.032608695652174</v>
       </c>
       <c r="C56">
-        <v>1134.475</v>
+        <v>1113.95</v>
       </c>
       <c r="D56">
-        <v>1240.2</v>
+        <v>1215.129032258065</v>
       </c>
       <c r="E56">
         <v>120</v>
@@ -1649,13 +1649,13 @@
         <v>59</v>
       </c>
       <c r="B57">
-        <v>1.854545454545454</v>
+        <v>1.818181818181818</v>
       </c>
       <c r="C57">
-        <v>804.4</v>
+        <v>806.775</v>
       </c>
       <c r="D57">
-        <v>1089.181818181818</v>
+        <v>1043.416666666667</v>
       </c>
       <c r="E57">
         <v>120</v>
@@ -1666,13 +1666,13 @@
         <v>60</v>
       </c>
       <c r="B58">
-        <v>1.911504424778761</v>
+        <v>1.902654867256637</v>
       </c>
       <c r="C58">
-        <v>1435.316666666667</v>
+        <v>1462.95</v>
       </c>
       <c r="D58">
-        <v>1098.686567164179</v>
+        <v>1074.640625</v>
       </c>
       <c r="E58">
         <v>120</v>
@@ -1683,16 +1683,16 @@
         <v>61</v>
       </c>
       <c r="B59">
-        <v>2.416666666666667</v>
+        <v>2.395833333333333</v>
       </c>
       <c r="C59">
-        <v>809.9591836734694</v>
+        <v>826.6799999999999</v>
       </c>
       <c r="D59">
         <v>1322.111111111111</v>
       </c>
       <c r="E59">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1700,13 +1700,13 @@
         <v>62</v>
       </c>
       <c r="B60">
-        <v>1.982142857142857</v>
+        <v>1.990990990990991</v>
       </c>
       <c r="C60">
-        <v>1290.924369747899</v>
+        <v>1290.571428571429</v>
       </c>
       <c r="D60">
-        <v>952.3529411764706</v>
+        <v>949.6666666666666</v>
       </c>
       <c r="E60">
         <v>120</v>
@@ -1717,13 +1717,13 @@
         <v>63</v>
       </c>
       <c r="B61">
-        <v>1.956521739130435</v>
+        <v>1.93859649122807</v>
       </c>
       <c r="C61">
-        <v>1133.058333333333</v>
+        <v>1205.579831932773</v>
       </c>
       <c r="D61">
-        <v>1059.375</v>
+        <v>1094.558823529412</v>
       </c>
       <c r="E61">
         <v>120</v>
@@ -1734,16 +1734,16 @@
         <v>64</v>
       </c>
       <c r="B62">
-        <v>2.125</v>
+        <v>2.137254901960784</v>
       </c>
       <c r="C62">
-        <v>887.3684210526316</v>
+        <v>898.7118644067797</v>
       </c>
       <c r="D62">
-        <v>1275.533333333333</v>
+        <v>1339.0625</v>
       </c>
       <c r="E62">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1751,13 +1751,13 @@
         <v>65</v>
       </c>
       <c r="B63">
-        <v>1.956521739130435</v>
+        <v>1.957264957264957</v>
       </c>
       <c r="C63">
-        <v>1086.975</v>
+        <v>1048.433333333333</v>
       </c>
       <c r="D63">
-        <v>1411.530612244898</v>
+        <v>1353.367346938775</v>
       </c>
       <c r="E63">
         <v>120</v>
@@ -1768,13 +1768,13 @@
         <v>66</v>
       </c>
       <c r="B64">
-        <v>1.725663716814159</v>
+        <v>1.752212389380531</v>
       </c>
       <c r="C64">
-        <v>850.9416666666667</v>
+        <v>853.2333333333333</v>
       </c>
       <c r="D64">
-        <v>756.697247706422</v>
+        <v>756.2962962962963</v>
       </c>
       <c r="E64">
         <v>120</v>
@@ -1785,13 +1785,13 @@
         <v>67</v>
       </c>
       <c r="B65">
-        <v>2.532110091743119</v>
+        <v>2.514285714285714</v>
       </c>
       <c r="C65">
-        <v>940.7563025210084</v>
+        <v>935.563025210084</v>
       </c>
       <c r="D65">
-        <v>1192.066666666667</v>
+        <v>1204.620689655172</v>
       </c>
       <c r="E65">
         <v>120</v>
@@ -1802,13 +1802,13 @@
         <v>68</v>
       </c>
       <c r="B66">
-        <v>2.194690265486726</v>
+        <v>2.165137614678899</v>
       </c>
       <c r="C66">
-        <v>1023.491666666667</v>
+        <v>996.0416666666666</v>
       </c>
       <c r="D66">
-        <v>1355.782608695652</v>
+        <v>1303.65306122449</v>
       </c>
       <c r="E66">
         <v>120</v>
@@ -1819,13 +1819,13 @@
         <v>69</v>
       </c>
       <c r="B67">
-        <v>2.180851063829787</v>
+        <v>2.231578947368421</v>
       </c>
       <c r="C67">
-        <v>1062.141666666667</v>
+        <v>1045.633333333333</v>
       </c>
       <c r="D67">
-        <v>914.934065934066</v>
+        <v>913</v>
       </c>
       <c r="E67">
         <v>120</v>
@@ -1836,13 +1836,13 @@
         <v>70</v>
       </c>
       <c r="B68">
-        <v>2.915789473684211</v>
+        <v>2.813725490196079</v>
       </c>
       <c r="C68">
-        <v>1532.283333333333</v>
+        <v>1726.591666666667</v>
       </c>
       <c r="D68">
-        <v>1306.571428571429</v>
+        <v>1985.157894736842</v>
       </c>
       <c r="E68">
         <v>120</v>
@@ -1853,16 +1853,16 @@
         <v>71</v>
       </c>
       <c r="B69">
-        <v>2.339285714285714</v>
+        <v>2.327272727272727</v>
       </c>
       <c r="C69">
-        <v>1025.852173913044</v>
+        <v>1022.169642857143</v>
       </c>
       <c r="D69">
-        <v>1184.666666666667</v>
+        <v>1169.319587628866</v>
       </c>
       <c r="E69">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1870,16 +1870,16 @@
         <v>72</v>
       </c>
       <c r="B70">
-        <v>2.067567567567568</v>
+        <v>2.081081081081081</v>
       </c>
       <c r="C70">
-        <v>1035.320512820513</v>
+        <v>1035.12987012987</v>
       </c>
       <c r="D70">
-        <v>1185.266666666667</v>
+        <v>1203.724137931034</v>
       </c>
       <c r="E70">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -1887,13 +1887,13 @@
         <v>73</v>
       </c>
       <c r="B71">
-        <v>1.906542056074766</v>
+        <v>1.878504672897196</v>
       </c>
       <c r="C71">
-        <v>938.2016806722689</v>
+        <v>932.109243697479</v>
       </c>
       <c r="D71">
-        <v>1174.483870967742</v>
+        <v>1173.064516129032</v>
       </c>
       <c r="E71">
         <v>120</v>
@@ -1904,13 +1904,13 @@
         <v>74</v>
       </c>
       <c r="B72">
-        <v>1.464285714285714</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="C72">
-        <v>1106.75</v>
+        <v>1155.302521008403</v>
       </c>
       <c r="D72">
-        <v>813.0547945205479</v>
+        <v>1017.625</v>
       </c>
       <c r="E72">
         <v>120</v>
@@ -1921,13 +1921,13 @@
         <v>75</v>
       </c>
       <c r="B73">
-        <v>1.577981651376147</v>
+        <v>1.55045871559633</v>
       </c>
       <c r="C73">
-        <v>869.4083333333333</v>
+        <v>863.15</v>
       </c>
       <c r="D73">
-        <v>787.0714285714286</v>
+        <v>787.3372093023256</v>
       </c>
       <c r="E73">
         <v>120</v>
@@ -1938,13 +1938,13 @@
         <v>76</v>
       </c>
       <c r="B74">
-        <v>1.85</v>
+        <v>1.841584158415842</v>
       </c>
       <c r="C74">
-        <v>1519.453781512605</v>
+        <v>1524.546218487395</v>
       </c>
       <c r="D74">
-        <v>1152.053191489362</v>
+        <v>1147.589473684211</v>
       </c>
       <c r="E74">
         <v>120</v>
@@ -1955,16 +1955,16 @@
         <v>77</v>
       </c>
       <c r="B75">
-        <v>2.222222222222222</v>
+        <v>2.241379310344827</v>
       </c>
       <c r="C75">
-        <v>1083.888888888889</v>
+        <v>1102.413793103448</v>
       </c>
       <c r="D75">
         <v>1371.722222222222</v>
       </c>
       <c r="E75">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1972,13 +1972,13 @@
         <v>78</v>
       </c>
       <c r="B76">
-        <v>1.823008849557522</v>
+        <v>1.818181818181818</v>
       </c>
       <c r="C76">
-        <v>1005.941176470588</v>
+        <v>1011.260504201681</v>
       </c>
       <c r="D76">
-        <v>1183.738461538461</v>
+        <v>1191.666666666667</v>
       </c>
       <c r="E76">
         <v>120</v>
@@ -1989,13 +1989,13 @@
         <v>79</v>
       </c>
       <c r="B77">
-        <v>1.485436893203884</v>
+        <v>1.462264150943396</v>
       </c>
       <c r="C77">
-        <v>1437.766666666667</v>
+        <v>1449.266666666667</v>
       </c>
       <c r="D77">
-        <v>804.5714285714286</v>
+        <v>833.8163265306123</v>
       </c>
       <c r="E77">
         <v>120</v>
@@ -2006,16 +2006,16 @@
         <v>80</v>
       </c>
       <c r="B78">
-        <v>1.875</v>
+        <v>1.884615384615385</v>
       </c>
       <c r="C78">
-        <v>781.625</v>
+        <v>819.1538461538462</v>
       </c>
       <c r="D78">
         <v>1124</v>
       </c>
       <c r="E78">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -2023,13 +2023,13 @@
         <v>81</v>
       </c>
       <c r="B79">
-        <v>2.287037037037037</v>
+        <v>2.292452830188679</v>
       </c>
       <c r="C79">
-        <v>1355.883333333333</v>
+        <v>1533.216666666667</v>
       </c>
       <c r="D79">
-        <v>889.4571428571429</v>
+        <v>976.6538461538462</v>
       </c>
       <c r="E79">
         <v>120</v>
@@ -2040,16 +2040,16 @@
         <v>82</v>
       </c>
       <c r="B80">
-        <v>2.166666666666667</v>
+        <v>2.181818181818182</v>
       </c>
       <c r="C80">
-        <v>906.75</v>
+        <v>914.6363636363636</v>
       </c>
       <c r="D80">
         <v>803.5555555555555</v>
       </c>
       <c r="E80">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -2057,13 +2057,13 @@
         <v>83</v>
       </c>
       <c r="B81">
-        <v>1.900900900900901</v>
+        <v>1.881818181818182</v>
       </c>
       <c r="C81">
-        <v>1250.915966386555</v>
+        <v>1256.344537815126</v>
       </c>
       <c r="D81">
-        <v>1429.846153846154</v>
+        <v>1418</v>
       </c>
       <c r="E81">
         <v>120</v>
@@ -2074,16 +2074,16 @@
         <v>84</v>
       </c>
       <c r="B82">
-        <v>1.794520547945206</v>
+        <v>1.773333333333333</v>
       </c>
       <c r="C82">
-        <v>793.1558441558442</v>
+        <v>789.9873417721519</v>
       </c>
       <c r="D82">
-        <v>930.0555555555555</v>
+        <v>919.7027027027027</v>
       </c>
       <c r="E82">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -2094,10 +2094,10 @@
         <v>1.747826086956522</v>
       </c>
       <c r="C83">
-        <v>1079.458333333333</v>
+        <v>1088.275</v>
       </c>
       <c r="D83">
-        <v>924.3166666666667</v>
+        <v>926.7903225806451</v>
       </c>
       <c r="E83">
         <v>120</v>
@@ -2108,16 +2108,16 @@
         <v>86</v>
       </c>
       <c r="B84">
-        <v>1.59375</v>
+        <v>1.553571428571429</v>
       </c>
       <c r="C84">
-        <v>1047.279411764706</v>
+        <v>1072.683333333333</v>
       </c>
       <c r="D84">
         <v>1351.222222222222</v>
       </c>
       <c r="E84">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -2125,13 +2125,13 @@
         <v>87</v>
       </c>
       <c r="B85">
-        <v>1.558558558558559</v>
+        <v>1.545454545454545</v>
       </c>
       <c r="C85">
-        <v>1401.083333333333</v>
+        <v>1410.408333333333</v>
       </c>
       <c r="D85">
-        <v>967.8928571428571</v>
+        <v>892.795918367347</v>
       </c>
       <c r="E85">
         <v>120</v>
@@ -2142,16 +2142,16 @@
         <v>88</v>
       </c>
       <c r="B86">
-        <v>1.662921348314607</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="C86">
-        <v>907.9191919191919</v>
+        <v>909.3200000000001</v>
       </c>
       <c r="D86">
-        <v>1151.925</v>
+        <v>1151.878048780488</v>
       </c>
       <c r="E86">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -2159,16 +2159,16 @@
         <v>89</v>
       </c>
       <c r="B87">
-        <v>2.063492063492064</v>
+        <v>2.116666666666667</v>
       </c>
       <c r="C87">
-        <v>913.8947368421053</v>
+        <v>910.6478873239437</v>
       </c>
       <c r="D87">
         <v>1222.5</v>
       </c>
       <c r="E87">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -2176,16 +2176,16 @@
         <v>90</v>
       </c>
       <c r="B88">
-        <v>2.070175438596491</v>
+        <v>2</v>
       </c>
       <c r="C88">
-        <v>817.1967213114754</v>
+        <v>812.6551724137931</v>
       </c>
       <c r="D88">
         <v>1029.294117647059</v>
       </c>
       <c r="E88">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -2193,16 +2193,16 @@
         <v>91</v>
       </c>
       <c r="B89">
-        <v>1.58695652173913</v>
+        <v>1.571428571428571</v>
       </c>
       <c r="C89">
-        <v>822.2786885245902</v>
+        <v>806.9677419354839</v>
       </c>
       <c r="D89">
-        <v>1077.368421052632</v>
+        <v>1079.315789473684</v>
       </c>
       <c r="E89">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -2210,13 +2210,13 @@
         <v>92</v>
       </c>
       <c r="B90">
-        <v>1.447368421052632</v>
+        <v>1.452173913043478</v>
       </c>
       <c r="C90">
-        <v>961.4333333333333</v>
+        <v>941.775</v>
       </c>
       <c r="D90">
-        <v>830.4197530864197</v>
+        <v>814.1375</v>
       </c>
       <c r="E90">
         <v>120</v>
@@ -2227,10 +2227,10 @@
         <v>93</v>
       </c>
       <c r="B91">
-        <v>3.108695652173913</v>
+        <v>3.130434782608696</v>
       </c>
       <c r="C91">
-        <v>2151.666666666667</v>
+        <v>2166.25</v>
       </c>
       <c r="D91">
         <v>1899.64705882353</v>
@@ -2244,16 +2244,16 @@
         <v>94</v>
       </c>
       <c r="B92">
-        <v>2.277777777777778</v>
+        <v>2.235294117647059</v>
       </c>
       <c r="C92">
-        <v>895.7894736842105</v>
+        <v>908.1764705882352</v>
       </c>
       <c r="D92">
-        <v>1682.5</v>
+        <v>1870</v>
       </c>
       <c r="E92">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -2261,13 +2261,13 @@
         <v>95</v>
       </c>
       <c r="B93">
-        <v>1.466666666666667</v>
+        <v>1.45</v>
       </c>
       <c r="C93">
-        <v>1245.583333333333</v>
+        <v>1251.625</v>
       </c>
       <c r="D93">
-        <v>870.0521739130435</v>
+        <v>866.9304347826087</v>
       </c>
       <c r="E93">
         <v>120</v>
@@ -2295,13 +2295,13 @@
         <v>97</v>
       </c>
       <c r="B95">
-        <v>3.191304347826087</v>
+        <v>3.156521739130435</v>
       </c>
       <c r="C95">
-        <v>1805.108333333333</v>
+        <v>1778.566666666667</v>
       </c>
       <c r="D95">
-        <v>1341.380952380952</v>
+        <v>2281.928571428572</v>
       </c>
       <c r="E95">
         <v>120</v>
@@ -2329,16 +2329,16 @@
         <v>99</v>
       </c>
       <c r="B97">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C97">
-        <v>1565</v>
+        <v>2000</v>
       </c>
       <c r="D97">
         <v>1700</v>
       </c>
       <c r="E97">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2363,10 +2363,10 @@
         <v>2</v>
       </c>
       <c r="C99">
-        <v>662.5</v>
+        <v>675</v>
       </c>
       <c r="E99">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -2391,13 +2391,13 @@
         <v>103</v>
       </c>
       <c r="B101">
-        <v>1.961538461538461</v>
+        <v>2.04</v>
       </c>
       <c r="C101">
-        <v>1264.827586206897</v>
+        <v>1225.172413793103</v>
       </c>
       <c r="D101">
-        <v>1244.133333333333</v>
+        <v>1247.285714285714</v>
       </c>
       <c r="E101">
         <v>29</v>
@@ -2408,16 +2408,16 @@
         <v>104</v>
       </c>
       <c r="B102">
-        <v>1.23728813559322</v>
+        <v>1.245614035087719</v>
       </c>
       <c r="C102">
-        <v>756.5333333333333</v>
+        <v>754.2586206896551</v>
       </c>
       <c r="D102">
-        <v>784</v>
+        <v>806.3333333333334</v>
       </c>
       <c r="E102">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -2456,16 +2456,16 @@
         <v>107</v>
       </c>
       <c r="B105">
-        <v>2.04</v>
+        <v>2.08695652173913</v>
       </c>
       <c r="C105">
-        <v>675.6060606060606</v>
+        <v>677.2903225806451</v>
       </c>
       <c r="D105">
         <v>883.3333333333334</v>
       </c>
       <c r="E105">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2473,16 +2473,16 @@
         <v>108</v>
       </c>
       <c r="B106">
-        <v>2.3</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="C106">
-        <v>717.5</v>
+        <v>730.5555555555555</v>
       </c>
       <c r="D106">
         <v>1200</v>
       </c>
       <c r="E106">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -2490,16 +2490,16 @@
         <v>109</v>
       </c>
       <c r="B107">
-        <v>1.807692307692308</v>
+        <v>1.8</v>
       </c>
       <c r="C107">
-        <v>742.7777777777778</v>
+        <v>742.5</v>
       </c>
       <c r="D107">
-        <v>877.7857142857143</v>
+        <v>879.5384615384615</v>
       </c>
       <c r="E107">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -2521,16 +2521,16 @@
         <v>111</v>
       </c>
       <c r="B109">
-        <v>1.82051282051282</v>
+        <v>1.804878048780488</v>
       </c>
       <c r="C109">
-        <v>795.275</v>
+        <v>778.2619047619048</v>
       </c>
       <c r="D109">
         <v>895.3</v>
       </c>
       <c r="E109">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -2538,16 +2538,16 @@
         <v>112</v>
       </c>
       <c r="B110">
-        <v>1.764705882352941</v>
+        <v>1.722222222222222</v>
       </c>
       <c r="C110">
-        <v>1508.857142857143</v>
+        <v>1517.027027027027</v>
       </c>
       <c r="D110">
-        <v>991.2857142857143</v>
+        <v>987.7333333333333</v>
       </c>
       <c r="E110">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -2572,16 +2572,16 @@
         <v>114</v>
       </c>
       <c r="B112">
-        <v>2.204081632653061</v>
+        <v>2.1875</v>
       </c>
       <c r="C112">
-        <v>785.6923076923077</v>
+        <v>782.9607843137255</v>
       </c>
       <c r="D112">
         <v>967.2</v>
       </c>
       <c r="E112">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -2603,16 +2603,16 @@
         <v>116</v>
       </c>
       <c r="B114">
-        <v>2.063829787234043</v>
+        <v>2.06</v>
       </c>
       <c r="C114">
-        <v>1597.88</v>
+        <v>1621.962264150943</v>
       </c>
       <c r="D114">
-        <v>1049.194444444444</v>
+        <v>1090.948717948718</v>
       </c>
       <c r="E114">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="115" spans="1:5">

</xml_diff>

<commit_message>
update to aggregate file
</commit_message>
<xml_diff>
--- a/AggregateCraigslistData.xlsx
+++ b/AggregateCraigslistData.xlsx
@@ -829,13 +829,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>1.541666666666667</v>
+        <v>1.533333333333333</v>
       </c>
       <c r="C7">
-        <v>958.8</v>
+        <v>957.8833333333333</v>
       </c>
       <c r="D7">
-        <v>974.1176470588235</v>
+        <v>969.5441176470588</v>
       </c>
       <c r="E7">
         <v>120</v>
@@ -846,16 +846,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>2.138888888888889</v>
+        <v>2.162162162162162</v>
       </c>
       <c r="C8">
-        <v>670.6666666666666</v>
+        <v>671.9302325581396</v>
       </c>
       <c r="D8">
         <v>874.1</v>
       </c>
       <c r="E8">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -939,7 +939,7 @@
         <v>2.537735849056604</v>
       </c>
       <c r="C14">
-        <v>652.9912280701755</v>
+        <v>653.1315789473684</v>
       </c>
       <c r="D14">
         <v>1113.941176470588</v>
@@ -1004,13 +1004,13 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>1.536363636363636</v>
+        <v>1.554545454545454</v>
       </c>
       <c r="C18">
-        <v>819.1949152542373</v>
+        <v>823.728813559322</v>
       </c>
       <c r="D18">
-        <v>827.4150943396227</v>
+        <v>840.9056603773585</v>
       </c>
       <c r="E18">
         <v>120</v>
@@ -1021,16 +1021,16 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>2.107142857142857</v>
+        <v>2.137931034482758</v>
       </c>
       <c r="C19">
-        <v>947.3548387096774</v>
+        <v>955.25</v>
       </c>
       <c r="D19">
         <v>1322.75</v>
       </c>
       <c r="E19">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1321,16 +1321,16 @@
         <v>39</v>
       </c>
       <c r="B37">
-        <v>1.639344262295082</v>
+        <v>1.645161290322581</v>
       </c>
       <c r="C37">
-        <v>610.8115942028985</v>
+        <v>611.0142857142857</v>
       </c>
       <c r="D37">
         <v>810.6</v>
       </c>
       <c r="E37">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1389,16 +1389,16 @@
         <v>43</v>
       </c>
       <c r="B41">
-        <v>2.065217391304348</v>
+        <v>2.085106382978724</v>
       </c>
       <c r="C41">
-        <v>667.8070175438596</v>
+        <v>666.6379310344828</v>
       </c>
       <c r="D41">
         <v>1253</v>
       </c>
       <c r="E41">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1474,16 +1474,16 @@
         <v>48</v>
       </c>
       <c r="B46">
-        <v>2.090909090909091</v>
+        <v>2.1</v>
       </c>
       <c r="C46">
-        <v>2855</v>
+        <v>3051.363636363636</v>
       </c>
       <c r="D46">
         <v>640</v>
       </c>
       <c r="E46">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1632,13 +1632,13 @@
         <v>58</v>
       </c>
       <c r="B56">
-        <v>2.032608695652174</v>
+        <v>2.043478260869565</v>
       </c>
       <c r="C56">
-        <v>1113.95</v>
+        <v>1126.033333333333</v>
       </c>
       <c r="D56">
-        <v>1215.129032258065</v>
+        <v>1236.516129032258</v>
       </c>
       <c r="E56">
         <v>120</v>
@@ -1666,13 +1666,13 @@
         <v>60</v>
       </c>
       <c r="B58">
-        <v>1.902654867256637</v>
+        <v>1.919642857142857</v>
       </c>
       <c r="C58">
-        <v>1462.95</v>
+        <v>1456.983333333333</v>
       </c>
       <c r="D58">
-        <v>1074.640625</v>
+        <v>1078.725806451613</v>
       </c>
       <c r="E58">
         <v>120</v>
@@ -1717,13 +1717,13 @@
         <v>63</v>
       </c>
       <c r="B61">
-        <v>1.93859649122807</v>
+        <v>1.929824561403509</v>
       </c>
       <c r="C61">
-        <v>1205.579831932773</v>
+        <v>1205.915966386555</v>
       </c>
       <c r="D61">
-        <v>1094.558823529412</v>
+        <v>1094.210526315789</v>
       </c>
       <c r="E61">
         <v>120</v>
@@ -1734,16 +1734,16 @@
         <v>64</v>
       </c>
       <c r="B62">
-        <v>2.137254901960784</v>
+        <v>2.150943396226415</v>
       </c>
       <c r="C62">
-        <v>898.7118644067797</v>
+        <v>907.7704918032787</v>
       </c>
       <c r="D62">
         <v>1339.0625</v>
       </c>
       <c r="E62">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1751,13 +1751,13 @@
         <v>65</v>
       </c>
       <c r="B63">
-        <v>1.957264957264957</v>
+        <v>1.965811965811966</v>
       </c>
       <c r="C63">
-        <v>1048.433333333333</v>
+        <v>1058.083333333333</v>
       </c>
       <c r="D63">
-        <v>1353.367346938775</v>
+        <v>1329.56862745098</v>
       </c>
       <c r="E63">
         <v>120</v>
@@ -1785,10 +1785,10 @@
         <v>67</v>
       </c>
       <c r="B65">
-        <v>2.514285714285714</v>
+        <v>2.495238095238095</v>
       </c>
       <c r="C65">
-        <v>935.563025210084</v>
+        <v>928.4201680672269</v>
       </c>
       <c r="D65">
         <v>1204.620689655172</v>
@@ -1802,13 +1802,13 @@
         <v>68</v>
       </c>
       <c r="B66">
-        <v>2.165137614678899</v>
+        <v>2.137614678899082</v>
       </c>
       <c r="C66">
-        <v>996.0416666666666</v>
+        <v>989.5916666666667</v>
       </c>
       <c r="D66">
-        <v>1303.65306122449</v>
+        <v>1290.58</v>
       </c>
       <c r="E66">
         <v>120</v>
@@ -1819,13 +1819,13 @@
         <v>69</v>
       </c>
       <c r="B67">
-        <v>2.231578947368421</v>
+        <v>2.252631578947368</v>
       </c>
       <c r="C67">
-        <v>1045.633333333333</v>
+        <v>1048.883333333333</v>
       </c>
       <c r="D67">
-        <v>913</v>
+        <v>915.8674698795181</v>
       </c>
       <c r="E67">
         <v>120</v>
@@ -1836,13 +1836,13 @@
         <v>70</v>
       </c>
       <c r="B68">
-        <v>2.813725490196079</v>
+        <v>2.861386138613861</v>
       </c>
       <c r="C68">
-        <v>1726.591666666667</v>
+        <v>1748.008333333333</v>
       </c>
       <c r="D68">
-        <v>1985.157894736842</v>
+        <v>1961.394736842105</v>
       </c>
       <c r="E68">
         <v>120</v>
@@ -1904,13 +1904,13 @@
         <v>74</v>
       </c>
       <c r="B72">
-        <v>1.666666666666667</v>
+        <v>1.663636363636364</v>
       </c>
       <c r="C72">
-        <v>1155.302521008403</v>
+        <v>1154.857142857143</v>
       </c>
       <c r="D72">
-        <v>1017.625</v>
+        <v>1016.214285714286</v>
       </c>
       <c r="E72">
         <v>120</v>
@@ -1924,7 +1924,7 @@
         <v>1.55045871559633</v>
       </c>
       <c r="C73">
-        <v>863.15</v>
+        <v>867.9083333333333</v>
       </c>
       <c r="D73">
         <v>787.3372093023256</v>
@@ -1938,13 +1938,13 @@
         <v>76</v>
       </c>
       <c r="B74">
-        <v>1.841584158415842</v>
+        <v>1.83</v>
       </c>
       <c r="C74">
-        <v>1524.546218487395</v>
+        <v>1512.747899159664</v>
       </c>
       <c r="D74">
-        <v>1147.589473684211</v>
+        <v>1133.410526315789</v>
       </c>
       <c r="E74">
         <v>120</v>
@@ -1955,16 +1955,16 @@
         <v>77</v>
       </c>
       <c r="B75">
-        <v>2.241379310344827</v>
+        <v>2.258064516129032</v>
       </c>
       <c r="C75">
-        <v>1102.413793103448</v>
+        <v>1100.290322580645</v>
       </c>
       <c r="D75">
         <v>1371.722222222222</v>
       </c>
       <c r="E75">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1989,13 +1989,13 @@
         <v>79</v>
       </c>
       <c r="B77">
-        <v>1.462264150943396</v>
+        <v>1.466666666666667</v>
       </c>
       <c r="C77">
-        <v>1449.266666666667</v>
+        <v>1446.533333333333</v>
       </c>
       <c r="D77">
-        <v>833.8163265306123</v>
+        <v>823.8571428571429</v>
       </c>
       <c r="E77">
         <v>120</v>
@@ -2026,10 +2026,10 @@
         <v>2.292452830188679</v>
       </c>
       <c r="C79">
-        <v>1533.216666666667</v>
+        <v>1530.208333333333</v>
       </c>
       <c r="D79">
-        <v>976.6538461538462</v>
+        <v>975.2075471698113</v>
       </c>
       <c r="E79">
         <v>120</v>
@@ -2091,13 +2091,13 @@
         <v>85</v>
       </c>
       <c r="B83">
-        <v>1.747826086956522</v>
+        <v>1.773913043478261</v>
       </c>
       <c r="C83">
-        <v>1088.275</v>
+        <v>1087.258333333333</v>
       </c>
       <c r="D83">
-        <v>926.7903225806451</v>
+        <v>940.65</v>
       </c>
       <c r="E83">
         <v>120</v>
@@ -2108,16 +2108,16 @@
         <v>86</v>
       </c>
       <c r="B84">
-        <v>1.553571428571429</v>
+        <v>1.56140350877193</v>
       </c>
       <c r="C84">
-        <v>1072.683333333333</v>
+        <v>1073.131147540984</v>
       </c>
       <c r="D84">
-        <v>1351.222222222222</v>
+        <v>1330.1</v>
       </c>
       <c r="E84">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -2128,10 +2128,10 @@
         <v>1.545454545454545</v>
       </c>
       <c r="C85">
-        <v>1410.408333333333</v>
+        <v>1407.616666666667</v>
       </c>
       <c r="D85">
-        <v>892.795918367347</v>
+        <v>916.8775510204082</v>
       </c>
       <c r="E85">
         <v>120</v>
@@ -2159,16 +2159,16 @@
         <v>89</v>
       </c>
       <c r="B87">
-        <v>2.116666666666667</v>
+        <v>2.114754098360656</v>
       </c>
       <c r="C87">
-        <v>910.6478873239437</v>
+        <v>911.0416666666666</v>
       </c>
       <c r="D87">
         <v>1222.5</v>
       </c>
       <c r="E87">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -2210,13 +2210,13 @@
         <v>92</v>
       </c>
       <c r="B90">
-        <v>1.452173913043478</v>
+        <v>1.469565217391304</v>
       </c>
       <c r="C90">
-        <v>941.775</v>
+        <v>945.9083333333333</v>
       </c>
       <c r="D90">
-        <v>814.1375</v>
+        <v>833.45</v>
       </c>
       <c r="E90">
         <v>120</v>
@@ -2261,13 +2261,13 @@
         <v>95</v>
       </c>
       <c r="B93">
-        <v>1.45</v>
+        <v>1.441666666666667</v>
       </c>
       <c r="C93">
-        <v>1251.625</v>
+        <v>1253.208333333333</v>
       </c>
       <c r="D93">
-        <v>866.9304347826087</v>
+        <v>864.4608695652174</v>
       </c>
       <c r="E93">
         <v>120</v>
@@ -2295,10 +2295,10 @@
         <v>97</v>
       </c>
       <c r="B95">
-        <v>3.156521739130435</v>
+        <v>3.146551724137931</v>
       </c>
       <c r="C95">
-        <v>1778.566666666667</v>
+        <v>1772.366666666667</v>
       </c>
       <c r="D95">
         <v>2281.928571428572</v>
@@ -2572,16 +2572,16 @@
         <v>114</v>
       </c>
       <c r="B112">
-        <v>2.1875</v>
+        <v>2.170212765957447</v>
       </c>
       <c r="C112">
-        <v>782.9607843137255</v>
+        <v>780.58</v>
       </c>
       <c r="D112">
         <v>967.2</v>
       </c>
       <c r="E112">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="113" spans="1:5">

</xml_diff>

<commit_message>
Update yelp data to excel
</commit_message>
<xml_diff>
--- a/AggregateCraigslistData.xlsx
+++ b/AggregateCraigslistData.xlsx
@@ -829,13 +829,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>1.533333333333333</v>
+        <v>1.516666666666667</v>
       </c>
       <c r="C7">
-        <v>969.425</v>
+        <v>964.8</v>
       </c>
       <c r="D7">
-        <v>974.9558823529412</v>
+        <v>967</v>
       </c>
       <c r="E7">
         <v>120</v>
@@ -936,10 +936,10 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>2.537735849056604</v>
+        <v>2.556603773584906</v>
       </c>
       <c r="C14">
-        <v>652.9473684210526</v>
+        <v>651.5877192982456</v>
       </c>
       <c r="D14">
         <v>1113.941176470588</v>
@@ -1021,16 +1021,16 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>2.166666666666667</v>
+        <v>2.193548387096774</v>
       </c>
       <c r="C19">
-        <v>916.3333333333334</v>
+        <v>924.6764705882352</v>
       </c>
       <c r="D19">
         <v>1322.75</v>
       </c>
       <c r="E19">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1273,16 +1273,16 @@
         <v>36</v>
       </c>
       <c r="B34">
-        <v>2.263157894736842</v>
+        <v>2.256410256410256</v>
       </c>
       <c r="C34">
-        <v>828.0952380952381</v>
+        <v>824.5348837209302</v>
       </c>
       <c r="D34">
-        <v>1269.473684210526</v>
+        <v>1256</v>
       </c>
       <c r="E34">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1491,16 +1491,16 @@
         <v>49</v>
       </c>
       <c r="B47">
-        <v>2.051546391752577</v>
+        <v>2.051020408163265</v>
       </c>
       <c r="C47">
-        <v>1078.724489795918</v>
+        <v>1080.707070707071</v>
       </c>
       <c r="D47">
-        <v>1045.647887323944</v>
+        <v>1045.625</v>
       </c>
       <c r="E47">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1641,13 +1641,13 @@
         <v>58</v>
       </c>
       <c r="B56">
-        <v>2.032608695652174</v>
+        <v>2.043478260869565</v>
       </c>
       <c r="C56">
-        <v>1117.241666666667</v>
+        <v>1123.075</v>
       </c>
       <c r="D56">
-        <v>1221.433333333333</v>
+        <v>1233.290322580645</v>
       </c>
       <c r="E56">
         <v>120</v>
@@ -1675,13 +1675,13 @@
         <v>60</v>
       </c>
       <c r="B58">
-        <v>1.919642857142857</v>
+        <v>1.929203539823009</v>
       </c>
       <c r="C58">
-        <v>1441.533333333333</v>
+        <v>1461.016666666667</v>
       </c>
       <c r="D58">
-        <v>1069.683333333333</v>
+        <v>1077.533333333333</v>
       </c>
       <c r="E58">
         <v>120</v>
@@ -1726,13 +1726,13 @@
         <v>63</v>
       </c>
       <c r="B61">
-        <v>1.982758620689655</v>
+        <v>2.008620689655173</v>
       </c>
       <c r="C61">
-        <v>1228.285714285714</v>
+        <v>1242.873949579832</v>
       </c>
       <c r="D61">
-        <v>1103.833333333333</v>
+        <v>1096.290322580645</v>
       </c>
       <c r="E61">
         <v>120</v>
@@ -1760,13 +1760,13 @@
         <v>65</v>
       </c>
       <c r="B63">
-        <v>1.949579831932773</v>
+        <v>1.957983193277311</v>
       </c>
       <c r="C63">
-        <v>1065.741666666667</v>
+        <v>1067.075</v>
       </c>
       <c r="D63">
-        <v>1341.511111111111</v>
+        <v>1345.212765957447</v>
       </c>
       <c r="E63">
         <v>120</v>
@@ -1780,10 +1780,10 @@
         <v>1.752212389380531</v>
       </c>
       <c r="C64">
-        <v>853.2333333333333</v>
+        <v>853.9416666666667</v>
       </c>
       <c r="D64">
-        <v>756.2962962962963</v>
+        <v>756.8518518518518</v>
       </c>
       <c r="E64">
         <v>120</v>
@@ -1828,13 +1828,13 @@
         <v>69</v>
       </c>
       <c r="B67">
-        <v>2.260416666666667</v>
+        <v>2.255102040816327</v>
       </c>
       <c r="C67">
-        <v>1045.908333333333</v>
+        <v>1045.15</v>
       </c>
       <c r="D67">
-        <v>923.4578313253012</v>
+        <v>927.2048192771084</v>
       </c>
       <c r="E67">
         <v>120</v>
@@ -1845,13 +1845,13 @@
         <v>70</v>
       </c>
       <c r="B68">
-        <v>2.95</v>
+        <v>2.92929292929293</v>
       </c>
       <c r="C68">
-        <v>1720.941666666667</v>
+        <v>1715.308333333333</v>
       </c>
       <c r="D68">
-        <v>1388.111111111111</v>
+        <v>1298.787878787879</v>
       </c>
       <c r="E68">
         <v>120</v>
@@ -1913,13 +1913,13 @@
         <v>74</v>
       </c>
       <c r="B72">
-        <v>1.585585585585586</v>
+        <v>1.567567567567568</v>
       </c>
       <c r="C72">
-        <v>1121.302521008403</v>
+        <v>1117.756302521008</v>
       </c>
       <c r="D72">
-        <v>1007.384615384615</v>
+        <v>990.0566037735849</v>
       </c>
       <c r="E72">
         <v>120</v>
@@ -1930,13 +1930,13 @@
         <v>75</v>
       </c>
       <c r="B73">
-        <v>1.532110091743119</v>
+        <v>1.522935779816514</v>
       </c>
       <c r="C73">
-        <v>865.2</v>
+        <v>864.2</v>
       </c>
       <c r="D73">
-        <v>787.7701149425287</v>
+        <v>786.8139534883721</v>
       </c>
       <c r="E73">
         <v>120</v>
@@ -1964,16 +1964,16 @@
         <v>77</v>
       </c>
       <c r="B75">
-        <v>2.233333333333333</v>
+        <v>2.258064516129032</v>
       </c>
       <c r="C75">
-        <v>1096.966666666667</v>
+        <v>1100.290322580645</v>
       </c>
       <c r="D75">
         <v>1371.722222222222</v>
       </c>
       <c r="E75">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1981,13 +1981,13 @@
         <v>78</v>
       </c>
       <c r="B76">
-        <v>1.8125</v>
+        <v>1.831858407079646</v>
       </c>
       <c r="C76">
-        <v>1006.458333333333</v>
+        <v>1010.15</v>
       </c>
       <c r="D76">
-        <v>1188.566037735849</v>
+        <v>1183.381818181818</v>
       </c>
       <c r="E76">
         <v>120</v>
@@ -1998,13 +1998,13 @@
         <v>79</v>
       </c>
       <c r="B77">
-        <v>1.407407407407407</v>
+        <v>1.445454545454546</v>
       </c>
       <c r="C77">
-        <v>1445.008333333333</v>
+        <v>1467.716666666667</v>
       </c>
       <c r="D77">
-        <v>814.2391304347826</v>
+        <v>839.5434782608696</v>
       </c>
       <c r="E77">
         <v>120</v>
@@ -2032,13 +2032,13 @@
         <v>81</v>
       </c>
       <c r="B79">
-        <v>2.323809523809524</v>
+        <v>2.355769230769231</v>
       </c>
       <c r="C79">
-        <v>1515.983333333333</v>
+        <v>1463.766666666667</v>
       </c>
       <c r="D79">
-        <v>971.36</v>
+        <v>961.9111111111112</v>
       </c>
       <c r="E79">
         <v>120</v>
@@ -2066,10 +2066,10 @@
         <v>83</v>
       </c>
       <c r="B81">
-        <v>1.9</v>
+        <v>1.909090909090909</v>
       </c>
       <c r="C81">
-        <v>1254.411764705882</v>
+        <v>1267.268907563025</v>
       </c>
       <c r="D81">
         <v>1423.333333333333</v>
@@ -2100,13 +2100,13 @@
         <v>85</v>
       </c>
       <c r="B83">
-        <v>1.739130434782609</v>
+        <v>1.756521739130435</v>
       </c>
       <c r="C83">
-        <v>1089.066666666667</v>
+        <v>1072.15</v>
       </c>
       <c r="D83">
-        <v>932.6842105263158</v>
+        <v>938.2962962962963</v>
       </c>
       <c r="E83">
         <v>120</v>
@@ -2134,13 +2134,13 @@
         <v>87</v>
       </c>
       <c r="B85">
-        <v>1.472727272727273</v>
+        <v>1.481818181818182</v>
       </c>
       <c r="C85">
-        <v>1362.533333333333</v>
+        <v>1380.866666666667</v>
       </c>
       <c r="D85">
-        <v>867.25</v>
+        <v>887.8039215686274</v>
       </c>
       <c r="E85">
         <v>120</v>
@@ -2168,16 +2168,16 @@
         <v>89</v>
       </c>
       <c r="B87">
-        <v>2.08695652173913</v>
+        <v>2.071428571428572</v>
       </c>
       <c r="C87">
-        <v>907.4</v>
+        <v>904.4074074074074</v>
       </c>
       <c r="D87">
         <v>1222.5</v>
       </c>
       <c r="E87">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -2202,16 +2202,16 @@
         <v>91</v>
       </c>
       <c r="B89">
-        <v>1.56</v>
+        <v>1.588235294117647</v>
       </c>
       <c r="C89">
-        <v>810.6666666666666</v>
+        <v>812.6875</v>
       </c>
       <c r="D89">
-        <v>1062.1</v>
+        <v>1047.857142857143</v>
       </c>
       <c r="E89">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -2222,10 +2222,10 @@
         <v>1.460869565217391</v>
       </c>
       <c r="C90">
-        <v>946.2416666666667</v>
+        <v>944.3666666666667</v>
       </c>
       <c r="D90">
-        <v>833.075</v>
+        <v>831.1375</v>
       </c>
       <c r="E90">
         <v>120</v>
@@ -2270,13 +2270,13 @@
         <v>95</v>
       </c>
       <c r="B93">
-        <v>1.45</v>
+        <v>1.425</v>
       </c>
       <c r="C93">
-        <v>1257.583333333333</v>
+        <v>1235.375</v>
       </c>
       <c r="D93">
-        <v>867.1304347826087</v>
+        <v>857.4347826086956</v>
       </c>
       <c r="E93">
         <v>120</v>
@@ -2304,10 +2304,10 @@
         <v>97</v>
       </c>
       <c r="B95">
-        <v>3.114035087719298</v>
+        <v>3.105263157894737</v>
       </c>
       <c r="C95">
-        <v>1784.85</v>
+        <v>1774.808333333333</v>
       </c>
       <c r="D95">
         <v>2234.275862068966</v>

</xml_diff>

<commit_message>
fixed yelp df issue
</commit_message>
<xml_diff>
--- a/AggregateCraigslistData.xlsx
+++ b/AggregateCraigslistData.xlsx
@@ -750,16 +750,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>2.055555555555555</v>
       </c>
       <c r="C2">
-        <v>1010.181818181818</v>
+        <v>1028.631578947368</v>
       </c>
       <c r="D2">
-        <v>985.5833333333334</v>
+        <v>1006.8</v>
       </c>
       <c r="E2">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -767,16 +767,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>2.038461538461538</v>
+        <v>1.92</v>
       </c>
       <c r="C3">
-        <v>746.6176470588235</v>
+        <v>666.969696969697</v>
       </c>
       <c r="D3">
-        <v>1335</v>
+        <v>1343.75</v>
       </c>
       <c r="E3">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -787,7 +787,7 @@
         <v>2.333333333333333</v>
       </c>
       <c r="C4">
-        <v>841.25</v>
+        <v>1020</v>
       </c>
       <c r="D4">
         <v>1042</v>
@@ -801,13 +801,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>1.75</v>
+        <v>1.833333333333333</v>
       </c>
       <c r="C5">
-        <v>735</v>
+        <v>780</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -829,13 +829,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>1.516666666666667</v>
+        <v>1.525</v>
       </c>
       <c r="C7">
-        <v>964.8</v>
+        <v>907.7666666666667</v>
       </c>
       <c r="D7">
-        <v>967</v>
+        <v>878.2321428571429</v>
       </c>
       <c r="E7">
         <v>120</v>
@@ -846,16 +846,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>2.157894736842105</v>
+        <v>2.171428571428571</v>
       </c>
       <c r="C8">
-        <v>670.2954545454545</v>
+        <v>662</v>
       </c>
       <c r="D8">
-        <v>874.1</v>
+        <v>889.7777777777778</v>
       </c>
       <c r="E8">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -863,16 +863,16 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>2.375</v>
+        <v>2.266666666666667</v>
       </c>
       <c r="C9">
-        <v>755.5555555555555</v>
+        <v>709.6875</v>
       </c>
       <c r="D9">
-        <v>1140</v>
+        <v>1100</v>
       </c>
       <c r="E9">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -897,16 +897,16 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>1.823529411764706</v>
+        <v>1.888888888888889</v>
       </c>
       <c r="C11">
-        <v>925.2941176470588</v>
+        <v>887.5</v>
       </c>
       <c r="D11">
         <v>1178</v>
       </c>
       <c r="E11">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -936,13 +936,13 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>2.556603773584906</v>
+        <v>2.642857142857143</v>
       </c>
       <c r="C14">
-        <v>651.5877192982456</v>
+        <v>575.8434782608696</v>
       </c>
       <c r="D14">
-        <v>1113.941176470588</v>
+        <v>1164.818181818182</v>
       </c>
       <c r="E14">
         <v>120</v>
@@ -953,16 +953,16 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>2.285714285714286</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="C15">
-        <v>842.8571428571429</v>
+        <v>858.8888888888889</v>
       </c>
       <c r="D15">
-        <v>1625</v>
+        <v>1650</v>
       </c>
       <c r="E15">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -970,16 +970,16 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>2.066666666666667</v>
+        <v>2.061224489795918</v>
       </c>
       <c r="C16">
-        <v>739.843137254902</v>
+        <v>727.8545454545455</v>
       </c>
       <c r="D16">
-        <v>917.8</v>
+        <v>897.9375</v>
       </c>
       <c r="E16">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -987,16 +987,16 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>3.666666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="C17">
-        <v>1616.666666666667</v>
+        <v>1448.75</v>
       </c>
       <c r="D17">
         <v>1500</v>
       </c>
       <c r="E17">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1004,13 +1004,13 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>1.554545454545454</v>
+        <v>1.564814814814815</v>
       </c>
       <c r="C18">
-        <v>816.0254237288135</v>
+        <v>826.8898305084746</v>
       </c>
       <c r="D18">
-        <v>845.1632653061224</v>
+        <v>914.9795918367347</v>
       </c>
       <c r="E18">
         <v>120</v>
@@ -1021,16 +1021,16 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>2.193548387096774</v>
+        <v>2.486486486486486</v>
       </c>
       <c r="C19">
-        <v>924.6764705882352</v>
+        <v>754.15</v>
       </c>
       <c r="D19">
-        <v>1322.75</v>
+        <v>1368.857142857143</v>
       </c>
       <c r="E19">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1038,16 +1038,16 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>1.538461538461539</v>
+        <v>1.571428571428571</v>
       </c>
       <c r="C20">
-        <v>520</v>
+        <v>531.0714285714286</v>
       </c>
       <c r="D20">
         <v>700</v>
       </c>
       <c r="E20">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1089,16 +1089,16 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>2.777777777777778</v>
+        <v>2.769230769230769</v>
       </c>
       <c r="C23">
-        <v>909</v>
+        <v>871.4285714285714</v>
       </c>
       <c r="D23">
-        <v>1063.333333333333</v>
+        <v>1047</v>
       </c>
       <c r="E23">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1106,16 +1106,16 @@
         <v>26</v>
       </c>
       <c r="B24">
-        <v>1.823529411764706</v>
+        <v>1.705882352941176</v>
       </c>
       <c r="C24">
-        <v>514.1</v>
+        <v>495.1052631578947</v>
       </c>
       <c r="D24">
-        <v>925</v>
+        <v>983.3333333333334</v>
       </c>
       <c r="E24">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1123,16 +1123,16 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>1.5</v>
+        <v>1.77027027027027</v>
       </c>
       <c r="C25">
-        <v>622</v>
+        <v>649.8076923076923</v>
       </c>
       <c r="D25">
-        <v>691.40625</v>
+        <v>707.8947368421053</v>
       </c>
       <c r="E25">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1140,16 +1140,16 @@
         <v>28</v>
       </c>
       <c r="B26">
-        <v>1.911111111111111</v>
+        <v>1.957446808510638</v>
       </c>
       <c r="C26">
-        <v>740.936170212766</v>
+        <v>743.48</v>
       </c>
       <c r="D26">
-        <v>979.6666666666666</v>
+        <v>971.8571428571429</v>
       </c>
       <c r="E26">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1157,16 +1157,16 @@
         <v>29</v>
       </c>
       <c r="B27">
-        <v>2.166666666666667</v>
+        <v>2.2</v>
       </c>
       <c r="C27">
-        <v>572.2222222222222</v>
+        <v>556.25</v>
       </c>
       <c r="D27">
         <v>1050</v>
       </c>
       <c r="E27">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1177,10 +1177,10 @@
         <v>2</v>
       </c>
       <c r="C28">
-        <v>858.25</v>
+        <v>894.3333333333334</v>
       </c>
       <c r="E28">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1188,13 +1188,13 @@
         <v>31</v>
       </c>
       <c r="B29">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="C29">
-        <v>1043.636363636364</v>
+        <v>1024.545454545455</v>
       </c>
       <c r="D29">
-        <v>1098</v>
+        <v>1101</v>
       </c>
       <c r="E29">
         <v>11</v>
@@ -1205,16 +1205,16 @@
         <v>32</v>
       </c>
       <c r="B30">
-        <v>2.133333333333333</v>
+        <v>1.928571428571429</v>
       </c>
       <c r="C30">
-        <v>660</v>
+        <v>644</v>
       </c>
       <c r="D30">
         <v>1125</v>
       </c>
       <c r="E30">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1222,16 +1222,16 @@
         <v>33</v>
       </c>
       <c r="B31">
-        <v>1.9375</v>
+        <v>1.933333333333333</v>
       </c>
       <c r="C31">
-        <v>870</v>
+        <v>863.8235294117648</v>
       </c>
       <c r="D31">
-        <v>1025.571428571429</v>
+        <v>1063.166666666667</v>
       </c>
       <c r="E31">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1256,16 +1256,16 @@
         <v>35</v>
       </c>
       <c r="B33">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="C33">
-        <v>1125</v>
+        <v>1138</v>
       </c>
       <c r="D33">
-        <v>1050</v>
+        <v>1375</v>
       </c>
       <c r="E33">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1273,16 +1273,16 @@
         <v>36</v>
       </c>
       <c r="B34">
-        <v>2.256410256410256</v>
+        <v>2.282051282051282</v>
       </c>
       <c r="C34">
-        <v>824.5348837209302</v>
+        <v>826</v>
       </c>
       <c r="D34">
-        <v>1256</v>
+        <v>1269.52380952381</v>
       </c>
       <c r="E34">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1290,16 +1290,16 @@
         <v>37</v>
       </c>
       <c r="B35">
-        <v>2.090909090909091</v>
+        <v>2.1</v>
       </c>
       <c r="C35">
-        <v>842.2727272727273</v>
+        <v>851.5</v>
       </c>
       <c r="D35">
         <v>1184.2</v>
       </c>
       <c r="E35">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1321,16 +1321,16 @@
         <v>39</v>
       </c>
       <c r="B37">
-        <v>1.65625</v>
+        <v>1.716417910447761</v>
       </c>
       <c r="C37">
-        <v>610.4305555555555</v>
+        <v>617.9736842105264</v>
       </c>
       <c r="D37">
-        <v>797.8085106382979</v>
+        <v>814.12</v>
       </c>
       <c r="E37">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1338,16 +1338,16 @@
         <v>40</v>
       </c>
       <c r="B38">
-        <v>1.846153846153846</v>
+        <v>1.909090909090909</v>
       </c>
       <c r="C38">
-        <v>1027.1875</v>
+        <v>1245.357142857143</v>
       </c>
       <c r="D38">
-        <v>1005</v>
+        <v>1150</v>
       </c>
       <c r="E38">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1358,7 +1358,7 @@
         <v>2.111111111111111</v>
       </c>
       <c r="C39">
-        <v>1350.5</v>
+        <v>1355.5</v>
       </c>
       <c r="D39">
         <v>1766.666666666667</v>
@@ -1372,16 +1372,16 @@
         <v>42</v>
       </c>
       <c r="B40">
-        <v>2.090909090909091</v>
+        <v>1.888888888888889</v>
       </c>
       <c r="C40">
-        <v>773.6363636363636</v>
+        <v>663.3333333333334</v>
       </c>
       <c r="D40">
-        <v>1000</v>
+        <v>833.3333333333334</v>
       </c>
       <c r="E40">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1389,13 +1389,13 @@
         <v>43</v>
       </c>
       <c r="B41">
-        <v>2.085106382978724</v>
+        <v>2.111111111111111</v>
       </c>
       <c r="C41">
-        <v>666.6379310344828</v>
+        <v>642.4137931034483</v>
       </c>
       <c r="D41">
-        <v>1253</v>
+        <v>1211.5</v>
       </c>
       <c r="E41">
         <v>60</v>
@@ -1406,16 +1406,16 @@
         <v>44</v>
       </c>
       <c r="B42">
-        <v>2.279069767441861</v>
+        <v>2.416666666666667</v>
       </c>
       <c r="C42">
-        <v>797.1190476190476</v>
+        <v>812.0857142857143</v>
       </c>
       <c r="D42">
-        <v>968.3181818181819</v>
+        <v>969.1428571428571</v>
       </c>
       <c r="E42">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1423,16 +1423,16 @@
         <v>45</v>
       </c>
       <c r="B43">
-        <v>1.878048780487805</v>
+        <v>1.896103896103896</v>
       </c>
       <c r="C43">
-        <v>683.1084337349398</v>
+        <v>683.8101265822785</v>
       </c>
       <c r="D43">
-        <v>1015.806451612903</v>
+        <v>1034.666666666667</v>
       </c>
       <c r="E43">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1440,13 +1440,10 @@
         <v>46</v>
       </c>
       <c r="B44">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="C44">
-        <v>723.3333333333334</v>
-      </c>
-      <c r="D44">
-        <v>1200</v>
+        <v>640</v>
       </c>
       <c r="E44">
         <v>4</v>
@@ -1457,16 +1454,16 @@
         <v>47</v>
       </c>
       <c r="B45">
-        <v>1.846153846153846</v>
+        <v>1.909090909090909</v>
       </c>
       <c r="C45">
-        <v>735</v>
+        <v>733.5714285714286</v>
       </c>
       <c r="D45">
-        <v>903.75</v>
+        <v>930</v>
       </c>
       <c r="E45">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1474,10 +1471,10 @@
         <v>48</v>
       </c>
       <c r="B46">
-        <v>2.1</v>
+        <v>2.090909090909091</v>
       </c>
       <c r="C46">
-        <v>3051.363636363636</v>
+        <v>3022.727272727273</v>
       </c>
       <c r="D46">
         <v>640</v>
@@ -1491,16 +1488,16 @@
         <v>49</v>
       </c>
       <c r="B47">
-        <v>2.051020408163265</v>
+        <v>2.009345794392523</v>
       </c>
       <c r="C47">
-        <v>1080.707070707071</v>
+        <v>1086.018518518518</v>
       </c>
       <c r="D47">
-        <v>1045.625</v>
+        <v>1033.876543209876</v>
       </c>
       <c r="E47">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1542,16 +1539,16 @@
         <v>52</v>
       </c>
       <c r="B50">
-        <v>2.115384615384615</v>
+        <v>2.107142857142857</v>
       </c>
       <c r="C50">
-        <v>784.8148148148148</v>
+        <v>807.4137931034483</v>
       </c>
       <c r="D50">
-        <v>1127.5</v>
+        <v>1074.285714285714</v>
       </c>
       <c r="E50">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1559,16 +1556,16 @@
         <v>53</v>
       </c>
       <c r="B51">
-        <v>2.072727272727273</v>
+        <v>2.083333333333333</v>
       </c>
       <c r="C51">
-        <v>668.0921052631579</v>
+        <v>661.2</v>
       </c>
       <c r="D51">
-        <v>1030</v>
+        <v>1085.5</v>
       </c>
       <c r="E51">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1576,16 +1573,16 @@
         <v>54</v>
       </c>
       <c r="B52">
-        <v>1.578947368421053</v>
+        <v>1.825</v>
       </c>
       <c r="C52">
-        <v>641.15625</v>
+        <v>665.0864197530864</v>
       </c>
       <c r="D52">
-        <v>800.8125</v>
+        <v>764.5599999999999</v>
       </c>
       <c r="E52">
-        <v>98</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1607,16 +1604,16 @@
         <v>56</v>
       </c>
       <c r="B54">
-        <v>1.90625</v>
+        <v>2.035714285714286</v>
       </c>
       <c r="C54">
-        <v>1135.75</v>
+        <v>1131</v>
       </c>
       <c r="D54">
-        <v>1172.642857142857</v>
+        <v>1236.416666666667</v>
       </c>
       <c r="E54">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1624,10 +1621,10 @@
         <v>57</v>
       </c>
       <c r="B55">
-        <v>2.064516129032258</v>
+        <v>2</v>
       </c>
       <c r="C55">
-        <v>653.1351351351351</v>
+        <v>675.5405405405405</v>
       </c>
       <c r="D55">
         <v>1100</v>
@@ -1641,13 +1638,13 @@
         <v>58</v>
       </c>
       <c r="B56">
-        <v>2.043478260869565</v>
+        <v>2.134146341463415</v>
       </c>
       <c r="C56">
-        <v>1123.075</v>
+        <v>1036.183333333333</v>
       </c>
       <c r="D56">
-        <v>1233.290322580645</v>
+        <v>1257.172413793103</v>
       </c>
       <c r="E56">
         <v>120</v>
@@ -1658,13 +1655,13 @@
         <v>59</v>
       </c>
       <c r="B57">
-        <v>1.850467289719626</v>
+        <v>1.968421052631579</v>
       </c>
       <c r="C57">
-        <v>801.2333333333333</v>
+        <v>763.325</v>
       </c>
       <c r="D57">
-        <v>1043.416666666667</v>
+        <v>1047.125</v>
       </c>
       <c r="E57">
         <v>120</v>
@@ -1675,13 +1672,13 @@
         <v>60</v>
       </c>
       <c r="B58">
-        <v>1.929203539823009</v>
+        <v>2.034782608695652</v>
       </c>
       <c r="C58">
-        <v>1461.016666666667</v>
+        <v>1519.75</v>
       </c>
       <c r="D58">
-        <v>1077.533333333333</v>
+        <v>1113.882352941177</v>
       </c>
       <c r="E58">
         <v>120</v>
@@ -1692,16 +1689,16 @@
         <v>61</v>
       </c>
       <c r="B59">
-        <v>2.408163265306122</v>
+        <v>2.375</v>
       </c>
       <c r="C59">
-        <v>818.6666666666666</v>
+        <v>803.1206896551724</v>
       </c>
       <c r="D59">
-        <v>1322.111111111111</v>
+        <v>1224.545454545455</v>
       </c>
       <c r="E59">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1709,13 +1706,13 @@
         <v>62</v>
       </c>
       <c r="B60">
-        <v>1.990990990990991</v>
+        <v>1.971698113207547</v>
       </c>
       <c r="C60">
-        <v>1291.613445378151</v>
+        <v>1253.705882352941</v>
       </c>
       <c r="D60">
-        <v>946.7058823529412</v>
+        <v>812.5</v>
       </c>
       <c r="E60">
         <v>120</v>
@@ -1726,13 +1723,13 @@
         <v>63</v>
       </c>
       <c r="B61">
-        <v>2.008620689655173</v>
+        <v>1.844036697247706</v>
       </c>
       <c r="C61">
-        <v>1242.873949579832</v>
+        <v>1174.076271186441</v>
       </c>
       <c r="D61">
-        <v>1096.290322580645</v>
+        <v>1016.125</v>
       </c>
       <c r="E61">
         <v>120</v>
@@ -1743,13 +1740,13 @@
         <v>64</v>
       </c>
       <c r="B62">
-        <v>2.122448979591837</v>
+        <v>2.347826086956522</v>
       </c>
       <c r="C62">
-        <v>884.1052631578947</v>
+        <v>887.8103448275862</v>
       </c>
       <c r="D62">
-        <v>1339.0625</v>
+        <v>1292.058823529412</v>
       </c>
       <c r="E62">
         <v>59</v>
@@ -1760,13 +1757,13 @@
         <v>65</v>
       </c>
       <c r="B63">
-        <v>1.957983193277311</v>
+        <v>1.939655172413793</v>
       </c>
       <c r="C63">
-        <v>1067.075</v>
+        <v>1090.741666666667</v>
       </c>
       <c r="D63">
-        <v>1345.212765957447</v>
+        <v>1298.88679245283</v>
       </c>
       <c r="E63">
         <v>120</v>
@@ -1780,10 +1777,10 @@
         <v>1.752212389380531</v>
       </c>
       <c r="C64">
-        <v>853.9416666666667</v>
+        <v>846.5833333333334</v>
       </c>
       <c r="D64">
-        <v>756.8518518518518</v>
+        <v>750.2857142857143</v>
       </c>
       <c r="E64">
         <v>120</v>
@@ -1794,16 +1791,16 @@
         <v>67</v>
       </c>
       <c r="B65">
-        <v>2.495238095238095</v>
+        <v>2.456521739130435</v>
       </c>
       <c r="C65">
-        <v>928.4201680672269</v>
+        <v>914.5631067961165</v>
       </c>
       <c r="D65">
-        <v>1204.620689655172</v>
+        <v>1207.259259259259</v>
       </c>
       <c r="E65">
-        <v>120</v>
+        <v>104</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1811,13 +1808,13 @@
         <v>68</v>
       </c>
       <c r="B66">
-        <v>2.128440366972477</v>
+        <v>2.194444444444445</v>
       </c>
       <c r="C66">
-        <v>980.4416666666667</v>
+        <v>991.45</v>
       </c>
       <c r="D66">
-        <v>1289.78431372549</v>
+        <v>1258.943396226415</v>
       </c>
       <c r="E66">
         <v>120</v>
@@ -1828,13 +1825,13 @@
         <v>69</v>
       </c>
       <c r="B67">
-        <v>2.255102040816327</v>
+        <v>2.313725490196079</v>
       </c>
       <c r="C67">
-        <v>1045.15</v>
+        <v>1012.966666666667</v>
       </c>
       <c r="D67">
-        <v>927.2048192771084</v>
+        <v>959.3493975903615</v>
       </c>
       <c r="E67">
         <v>120</v>
@@ -1845,13 +1842,13 @@
         <v>70</v>
       </c>
       <c r="B68">
-        <v>2.92929292929293</v>
+        <v>3.168316831683168</v>
       </c>
       <c r="C68">
-        <v>1715.308333333333</v>
+        <v>1805.666666666667</v>
       </c>
       <c r="D68">
-        <v>1298.787878787879</v>
+        <v>1058.727272727273</v>
       </c>
       <c r="E68">
         <v>120</v>
@@ -1862,16 +1859,16 @@
         <v>71</v>
       </c>
       <c r="B69">
-        <v>2.327272727272727</v>
+        <v>2.485436893203883</v>
       </c>
       <c r="C69">
-        <v>1021.589285714286</v>
+        <v>1049.792452830189</v>
       </c>
       <c r="D69">
-        <v>1169.319587628866</v>
+        <v>1217.031578947368</v>
       </c>
       <c r="E69">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1879,16 +1876,16 @@
         <v>72</v>
       </c>
       <c r="B70">
-        <v>2.081081081081081</v>
+        <v>2.0625</v>
       </c>
       <c r="C70">
-        <v>1042.171052631579</v>
+        <v>1047.25</v>
       </c>
       <c r="D70">
-        <v>1203.724137931034</v>
+        <v>1206.826086956522</v>
       </c>
       <c r="E70">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -1896,13 +1893,13 @@
         <v>73</v>
       </c>
       <c r="B71">
-        <v>1.833333333333333</v>
+        <v>1.853211009174312</v>
       </c>
       <c r="C71">
-        <v>924.1176470588235</v>
+        <v>931.0252100840336</v>
       </c>
       <c r="D71">
-        <v>1140.5</v>
+        <v>1208.259259259259</v>
       </c>
       <c r="E71">
         <v>120</v>
@@ -1913,13 +1910,13 @@
         <v>74</v>
       </c>
       <c r="B72">
-        <v>1.567567567567568</v>
+        <v>1.766666666666667</v>
       </c>
       <c r="C72">
-        <v>1117.756302521008</v>
+        <v>1243.083333333333</v>
       </c>
       <c r="D72">
-        <v>990.0566037735849</v>
+        <v>952.9636363636364</v>
       </c>
       <c r="E72">
         <v>120</v>
@@ -1930,13 +1927,13 @@
         <v>75</v>
       </c>
       <c r="B73">
-        <v>1.522935779816514</v>
+        <v>1.548672566371681</v>
       </c>
       <c r="C73">
-        <v>864.2</v>
+        <v>846.7666666666667</v>
       </c>
       <c r="D73">
-        <v>786.8139534883721</v>
+        <v>788.05</v>
       </c>
       <c r="E73">
         <v>120</v>
@@ -1947,13 +1944,13 @@
         <v>76</v>
       </c>
       <c r="B74">
-        <v>1.821782178217822</v>
+        <v>1.833333333333333</v>
       </c>
       <c r="C74">
-        <v>1520.563025210084</v>
+        <v>1510.991666666667</v>
       </c>
       <c r="D74">
-        <v>1147.589473684211</v>
+        <v>1168.397959183673</v>
       </c>
       <c r="E74">
         <v>120</v>
@@ -1964,16 +1961,16 @@
         <v>77</v>
       </c>
       <c r="B75">
-        <v>2.258064516129032</v>
+        <v>2.275862068965517</v>
       </c>
       <c r="C75">
-        <v>1100.290322580645</v>
+        <v>1105.466666666667</v>
       </c>
       <c r="D75">
-        <v>1371.722222222222</v>
+        <v>1348.411764705882</v>
       </c>
       <c r="E75">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1981,13 +1978,13 @@
         <v>78</v>
       </c>
       <c r="B76">
-        <v>1.831858407079646</v>
+        <v>1.821428571428571</v>
       </c>
       <c r="C76">
-        <v>1010.15</v>
+        <v>970.9747899159664</v>
       </c>
       <c r="D76">
-        <v>1183.381818181818</v>
+        <v>1139.5</v>
       </c>
       <c r="E76">
         <v>120</v>
@@ -1998,13 +1995,13 @@
         <v>79</v>
       </c>
       <c r="B77">
-        <v>1.445454545454546</v>
+        <v>1.514285714285714</v>
       </c>
       <c r="C77">
-        <v>1467.716666666667</v>
+        <v>1416.641666666667</v>
       </c>
       <c r="D77">
-        <v>839.5434782608696</v>
+        <v>777.7843137254902</v>
       </c>
       <c r="E77">
         <v>120</v>
@@ -2018,7 +2015,7 @@
         <v>1.884615384615385</v>
       </c>
       <c r="C78">
-        <v>819.1538461538462</v>
+        <v>798</v>
       </c>
       <c r="D78">
         <v>1124</v>
@@ -2032,13 +2029,13 @@
         <v>81</v>
       </c>
       <c r="B79">
-        <v>2.355769230769231</v>
+        <v>2.26605504587156</v>
       </c>
       <c r="C79">
-        <v>1463.766666666667</v>
+        <v>1524.725</v>
       </c>
       <c r="D79">
-        <v>961.9111111111112</v>
+        <v>975.0204081632653</v>
       </c>
       <c r="E79">
         <v>120</v>
@@ -2049,16 +2046,16 @@
         <v>82</v>
       </c>
       <c r="B80">
-        <v>2.181818181818182</v>
+        <v>2</v>
       </c>
       <c r="C80">
-        <v>914.6363636363636</v>
+        <v>876.6</v>
       </c>
       <c r="D80">
-        <v>803.5555555555555</v>
+        <v>664.75</v>
       </c>
       <c r="E80">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -2066,13 +2063,13 @@
         <v>83</v>
       </c>
       <c r="B81">
-        <v>1.909090909090909</v>
+        <v>1.927272727272727</v>
       </c>
       <c r="C81">
-        <v>1267.268907563025</v>
+        <v>1275.739495798319</v>
       </c>
       <c r="D81">
-        <v>1423.333333333333</v>
+        <v>1452.272727272727</v>
       </c>
       <c r="E81">
         <v>120</v>
@@ -2083,16 +2080,16 @@
         <v>84</v>
       </c>
       <c r="B82">
-        <v>1.773333333333333</v>
+        <v>1.816901408450704</v>
       </c>
       <c r="C82">
-        <v>789.9873417721519</v>
+        <v>773.5</v>
       </c>
       <c r="D82">
-        <v>919.7027027027027</v>
+        <v>866.5555555555555</v>
       </c>
       <c r="E82">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -2100,13 +2097,13 @@
         <v>85</v>
       </c>
       <c r="B83">
-        <v>1.756521739130435</v>
+        <v>1.732758620689655</v>
       </c>
       <c r="C83">
-        <v>1072.15</v>
+        <v>1037.308333333333</v>
       </c>
       <c r="D83">
-        <v>938.2962962962963</v>
+        <v>925.2916666666666</v>
       </c>
       <c r="E83">
         <v>120</v>
@@ -2117,16 +2114,16 @@
         <v>86</v>
       </c>
       <c r="B84">
-        <v>1.56140350877193</v>
+        <v>1.566666666666667</v>
       </c>
       <c r="C84">
-        <v>1073.131147540984</v>
+        <v>1062.515625</v>
       </c>
       <c r="D84">
-        <v>1330.1</v>
+        <v>1303.923076923077</v>
       </c>
       <c r="E84">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -2134,13 +2131,13 @@
         <v>87</v>
       </c>
       <c r="B85">
-        <v>1.481818181818182</v>
+        <v>1.693693693693694</v>
       </c>
       <c r="C85">
-        <v>1380.866666666667</v>
+        <v>1405.116666666667</v>
       </c>
       <c r="D85">
-        <v>887.8039215686274</v>
+        <v>917.4222222222222</v>
       </c>
       <c r="E85">
         <v>120</v>
@@ -2151,16 +2148,16 @@
         <v>88</v>
       </c>
       <c r="B86">
-        <v>1.662921348314607</v>
+        <v>1.717391304347826</v>
       </c>
       <c r="C86">
-        <v>906.3838383838383</v>
+        <v>872.5436893203884</v>
       </c>
       <c r="D86">
-        <v>1150.675</v>
+        <v>1187.694444444444</v>
       </c>
       <c r="E86">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -2168,16 +2165,16 @@
         <v>89</v>
       </c>
       <c r="B87">
-        <v>2.071428571428572</v>
+        <v>2.050632911392405</v>
       </c>
       <c r="C87">
-        <v>904.4074074074074</v>
+        <v>877.3820224719101</v>
       </c>
       <c r="D87">
-        <v>1222.5</v>
+        <v>1189.166666666667</v>
       </c>
       <c r="E87">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -2185,13 +2182,13 @@
         <v>90</v>
       </c>
       <c r="B88">
-        <v>2.018181818181818</v>
+        <v>2.018867924528302</v>
       </c>
       <c r="C88">
-        <v>819.6440677966102</v>
+        <v>779.6896551724138</v>
       </c>
       <c r="D88">
-        <v>1029.294117647059</v>
+        <v>962.3571428571429</v>
       </c>
       <c r="E88">
         <v>59</v>
@@ -2202,16 +2199,16 @@
         <v>91</v>
       </c>
       <c r="B89">
-        <v>1.588235294117647</v>
+        <v>1.795454545454545</v>
       </c>
       <c r="C89">
-        <v>812.6875</v>
+        <v>872.0862068965517</v>
       </c>
       <c r="D89">
-        <v>1047.857142857143</v>
+        <v>1049.625</v>
       </c>
       <c r="E89">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -2219,13 +2216,13 @@
         <v>92</v>
       </c>
       <c r="B90">
-        <v>1.460869565217391</v>
+        <v>1.482758620689655</v>
       </c>
       <c r="C90">
-        <v>944.3666666666667</v>
+        <v>3124.116666666667</v>
       </c>
       <c r="D90">
-        <v>831.1375</v>
+        <v>887.7564102564103</v>
       </c>
       <c r="E90">
         <v>120</v>
@@ -2236,16 +2233,16 @@
         <v>93</v>
       </c>
       <c r="B91">
-        <v>3.130434782608696</v>
+        <v>3.240740740740741</v>
       </c>
       <c r="C91">
-        <v>2166.25</v>
+        <v>2227.363636363636</v>
       </c>
       <c r="D91">
-        <v>1899.64705882353</v>
+        <v>1910</v>
       </c>
       <c r="E91">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -2253,16 +2250,16 @@
         <v>94</v>
       </c>
       <c r="B92">
-        <v>2.235294117647059</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="C92">
-        <v>908.1764705882352</v>
+        <v>878.2777777777778</v>
       </c>
       <c r="D92">
         <v>1870</v>
       </c>
       <c r="E92">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -2270,13 +2267,13 @@
         <v>95</v>
       </c>
       <c r="B93">
-        <v>1.425</v>
+        <v>1.391666666666667</v>
       </c>
       <c r="C93">
-        <v>1235.375</v>
+        <v>1226.083333333333</v>
       </c>
       <c r="D93">
-        <v>857.4347826086956</v>
+        <v>839.2222222222222</v>
       </c>
       <c r="E93">
         <v>120</v>
@@ -2287,16 +2284,16 @@
         <v>96</v>
       </c>
       <c r="B94">
-        <v>2.176470588235294</v>
+        <v>2.133333333333333</v>
       </c>
       <c r="C94">
-        <v>1206.578947368421</v>
+        <v>1273.611111111111</v>
       </c>
       <c r="D94">
-        <v>1860.375</v>
+        <v>1840.333333333333</v>
       </c>
       <c r="E94">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -2304,13 +2301,13 @@
         <v>97</v>
       </c>
       <c r="B95">
-        <v>3.105263157894737</v>
+        <v>3.130434782608696</v>
       </c>
       <c r="C95">
-        <v>1774.808333333333</v>
+        <v>1783.941666666667</v>
       </c>
       <c r="D95">
-        <v>2234.275862068966</v>
+        <v>2449.125</v>
       </c>
       <c r="E95">
         <v>120</v>
@@ -2372,10 +2369,10 @@
         <v>2</v>
       </c>
       <c r="C99">
-        <v>675</v>
+        <v>812.5</v>
       </c>
       <c r="E99">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -2400,13 +2397,13 @@
         <v>103</v>
       </c>
       <c r="B101">
-        <v>2.04</v>
+        <v>2.16</v>
       </c>
       <c r="C101">
-        <v>1225.172413793103</v>
+        <v>1276.551724137931</v>
       </c>
       <c r="D101">
-        <v>1247.285714285714</v>
+        <v>1250.333333333333</v>
       </c>
       <c r="E101">
         <v>29</v>
@@ -2417,16 +2414,16 @@
         <v>104</v>
       </c>
       <c r="B102">
-        <v>1.245614035087719</v>
+        <v>1.265625</v>
       </c>
       <c r="C102">
-        <v>754</v>
+        <v>749.1076923076923</v>
       </c>
       <c r="D102">
-        <v>806.3333333333334</v>
+        <v>800.4615384615385</v>
       </c>
       <c r="E102">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -2434,7 +2431,7 @@
         <v>105</v>
       </c>
       <c r="B103">
-        <v>1.714285714285714</v>
+        <v>1.571428571428571</v>
       </c>
       <c r="C103">
         <v>735</v>
@@ -2451,13 +2448,13 @@
         <v>106</v>
       </c>
       <c r="B104">
-        <v>2.333333333333333</v>
+        <v>2</v>
       </c>
       <c r="C104">
-        <v>1187.5</v>
+        <v>1200</v>
       </c>
       <c r="E104">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -2465,16 +2462,16 @@
         <v>107</v>
       </c>
       <c r="B105">
-        <v>2.08695652173913</v>
+        <v>1.952380952380952</v>
       </c>
       <c r="C105">
-        <v>677.2903225806451</v>
+        <v>682</v>
       </c>
       <c r="D105">
-        <v>883.3333333333334</v>
+        <v>855</v>
       </c>
       <c r="E105">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2499,16 +2496,16 @@
         <v>109</v>
       </c>
       <c r="B107">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="C107">
-        <v>742.5</v>
+        <v>785.3571428571429</v>
       </c>
       <c r="D107">
-        <v>879.5384615384615</v>
+        <v>1052</v>
       </c>
       <c r="E107">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -2530,13 +2527,13 @@
         <v>111</v>
       </c>
       <c r="B109">
-        <v>1.804878048780488</v>
+        <v>1.829268292682927</v>
       </c>
       <c r="C109">
-        <v>778.2619047619048</v>
+        <v>797.9047619047619</v>
       </c>
       <c r="D109">
-        <v>895.3</v>
+        <v>950.25</v>
       </c>
       <c r="E109">
         <v>43</v>
@@ -2547,16 +2544,16 @@
         <v>112</v>
       </c>
       <c r="B110">
-        <v>1.742857142857143</v>
+        <v>1.621621621621622</v>
       </c>
       <c r="C110">
-        <v>1534.305555555556</v>
+        <v>1565.263157894737</v>
       </c>
       <c r="D110">
-        <v>997.6551724137931</v>
+        <v>978.516129032258</v>
       </c>
       <c r="E110">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -2564,16 +2561,16 @@
         <v>113</v>
       </c>
       <c r="B111">
-        <v>2.230769230769231</v>
+        <v>2.1875</v>
       </c>
       <c r="C111">
-        <v>762.0714285714286</v>
+        <v>733.1764705882352</v>
       </c>
       <c r="D111">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="E111">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -2581,13 +2578,13 @@
         <v>114</v>
       </c>
       <c r="B112">
-        <v>2.170212765957447</v>
+        <v>2.217391304347826</v>
       </c>
       <c r="C112">
-        <v>780.58</v>
+        <v>781.7254901960785</v>
       </c>
       <c r="D112">
-        <v>967.2</v>
+        <v>992.1904761904761</v>
       </c>
       <c r="E112">
         <v>51</v>
@@ -2598,13 +2595,16 @@
         <v>115</v>
       </c>
       <c r="B113">
-        <v>2</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="C113">
-        <v>525</v>
+        <v>575</v>
+      </c>
+      <c r="D113">
+        <v>1700</v>
       </c>
       <c r="E113">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -2612,16 +2612,16 @@
         <v>116</v>
       </c>
       <c r="B114">
-        <v>2.06</v>
+        <v>1.925925925925926</v>
       </c>
       <c r="C114">
-        <v>1621.962264150943</v>
+        <v>1643.070175438596</v>
       </c>
       <c r="D114">
-        <v>1090.948717948718</v>
+        <v>1102.068181818182</v>
       </c>
       <c r="E114">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -2629,16 +2629,16 @@
         <v>117</v>
       </c>
       <c r="B115">
-        <v>2.5</v>
+        <v>2.222222222222222</v>
       </c>
       <c r="C115">
-        <v>786</v>
+        <v>751.8181818181819</v>
       </c>
       <c r="D115">
-        <v>1000</v>
+        <v>933.3333333333334</v>
       </c>
       <c r="E115">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added price plot file
</commit_message>
<xml_diff>
--- a/AggregateCraigslistData.xlsx
+++ b/AggregateCraigslistData.xlsx
@@ -750,16 +750,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>2.055555555555555</v>
+        <v>2.105263157894737</v>
       </c>
       <c r="C2">
-        <v>1028.631578947368</v>
+        <v>1025.2</v>
       </c>
       <c r="D2">
-        <v>1006.8</v>
+        <v>1006.6</v>
       </c>
       <c r="E2">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -767,16 +767,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>1.92</v>
+        <v>1.88</v>
       </c>
       <c r="C3">
-        <v>666.969696969697</v>
+        <v>649.375</v>
       </c>
       <c r="D3">
-        <v>1343.75</v>
+        <v>1550</v>
       </c>
       <c r="E3">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -784,16 +784,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>2.333333333333333</v>
+        <v>2.166666666666667</v>
       </c>
       <c r="C4">
-        <v>1020</v>
+        <v>887.1428571428571</v>
       </c>
       <c r="D4">
-        <v>1042</v>
+        <v>1094.666666666667</v>
       </c>
       <c r="E4">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -801,13 +801,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>1.833333333333333</v>
+        <v>1.6</v>
       </c>
       <c r="C5">
-        <v>780</v>
+        <v>746</v>
       </c>
       <c r="E5">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -829,13 +829,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>1.525</v>
+        <v>1.508333333333333</v>
       </c>
       <c r="C7">
-        <v>907.7666666666667</v>
+        <v>865.325</v>
       </c>
       <c r="D7">
-        <v>878.2321428571429</v>
+        <v>880.625</v>
       </c>
       <c r="E7">
         <v>120</v>
@@ -846,16 +846,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>2.171428571428571</v>
+        <v>2.179487179487179</v>
       </c>
       <c r="C8">
-        <v>662</v>
+        <v>667.5714285714286</v>
       </c>
       <c r="D8">
-        <v>889.7777777777778</v>
+        <v>874.1</v>
       </c>
       <c r="E8">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -866,10 +866,10 @@
         <v>2.266666666666667</v>
       </c>
       <c r="C9">
-        <v>709.6875</v>
+        <v>717.5</v>
       </c>
       <c r="D9">
-        <v>1100</v>
+        <v>1130</v>
       </c>
       <c r="E9">
         <v>19</v>
@@ -880,13 +880,13 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="C10">
-        <v>1750</v>
+        <v>2000</v>
       </c>
       <c r="D10">
-        <v>1550</v>
+        <v>2000</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -900,7 +900,7 @@
         <v>1.888888888888889</v>
       </c>
       <c r="C11">
-        <v>887.5</v>
+        <v>887.2222222222222</v>
       </c>
       <c r="D11">
         <v>1178</v>
@@ -936,13 +936,13 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>2.642857142857143</v>
+        <v>2.734513274336283</v>
       </c>
       <c r="C14">
-        <v>575.8434782608696</v>
+        <v>569.1769911504425</v>
       </c>
       <c r="D14">
-        <v>1164.818181818182</v>
+        <v>1328</v>
       </c>
       <c r="E14">
         <v>120</v>
@@ -956,13 +956,13 @@
         <v>2.333333333333333</v>
       </c>
       <c r="C15">
-        <v>858.8888888888889</v>
+        <v>867.5</v>
       </c>
       <c r="D15">
-        <v>1650</v>
+        <v>1600</v>
       </c>
       <c r="E15">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -970,16 +970,16 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>2.061224489795918</v>
+        <v>2.071428571428572</v>
       </c>
       <c r="C16">
-        <v>727.8545454545455</v>
+        <v>736.1020408163265</v>
       </c>
       <c r="D16">
-        <v>897.9375</v>
+        <v>889.1538461538462</v>
       </c>
       <c r="E16">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -987,16 +987,16 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="C17">
-        <v>1448.75</v>
+        <v>1279</v>
       </c>
       <c r="D17">
-        <v>1500</v>
+        <v>1240</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1004,13 +1004,13 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>1.564814814814815</v>
+        <v>1.555555555555556</v>
       </c>
       <c r="C18">
-        <v>826.8898305084746</v>
+        <v>824.8559322033898</v>
       </c>
       <c r="D18">
-        <v>914.9795918367347</v>
+        <v>902.8367346938776</v>
       </c>
       <c r="E18">
         <v>120</v>
@@ -1021,16 +1021,16 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>2.486486486486486</v>
+        <v>2.543478260869565</v>
       </c>
       <c r="C19">
-        <v>754.15</v>
+        <v>688.0943396226415</v>
       </c>
       <c r="D19">
         <v>1368.857142857143</v>
       </c>
       <c r="E19">
-        <v>40</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1038,16 +1038,16 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>1.571428571428571</v>
+        <v>1.538461538461539</v>
       </c>
       <c r="C20">
-        <v>531.0714285714286</v>
+        <v>518.0769230769231</v>
       </c>
       <c r="D20">
         <v>700</v>
       </c>
       <c r="E20">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1055,16 +1055,16 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>2.666666666666667</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="C21">
-        <v>1203.333333333333</v>
+        <v>891.6666666666666</v>
       </c>
       <c r="D21">
-        <v>1474.4</v>
+        <v>1270</v>
       </c>
       <c r="E21">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1089,16 +1089,16 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>2.769230769230769</v>
+        <v>2.714285714285714</v>
       </c>
       <c r="C23">
-        <v>871.4285714285714</v>
+        <v>856.6666666666666</v>
       </c>
       <c r="D23">
         <v>1047</v>
       </c>
       <c r="E23">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1106,16 +1106,16 @@
         <v>26</v>
       </c>
       <c r="B24">
-        <v>1.705882352941176</v>
+        <v>1.764705882352941</v>
       </c>
       <c r="C24">
-        <v>495.1052631578947</v>
+        <v>511.7777777777778</v>
       </c>
       <c r="D24">
         <v>983.3333333333334</v>
       </c>
       <c r="E24">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1123,16 +1123,16 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>1.77027027027027</v>
+        <v>1.794871794871795</v>
       </c>
       <c r="C25">
-        <v>649.8076923076923</v>
+        <v>647.1927710843373</v>
       </c>
       <c r="D25">
-        <v>707.8947368421053</v>
+        <v>754.7619047619048</v>
       </c>
       <c r="E25">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1140,13 +1140,13 @@
         <v>28</v>
       </c>
       <c r="B26">
-        <v>1.957446808510638</v>
+        <v>1.914893617021277</v>
       </c>
       <c r="C26">
-        <v>743.48</v>
+        <v>739.48</v>
       </c>
       <c r="D26">
-        <v>971.8571428571429</v>
+        <v>903.5</v>
       </c>
       <c r="E26">
         <v>50</v>
@@ -1157,16 +1157,16 @@
         <v>29</v>
       </c>
       <c r="B27">
-        <v>2.2</v>
+        <v>2.25</v>
       </c>
       <c r="C27">
-        <v>556.25</v>
+        <v>535.7142857142857</v>
       </c>
       <c r="D27">
         <v>1050</v>
       </c>
       <c r="E27">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1177,10 +1177,10 @@
         <v>2</v>
       </c>
       <c r="C28">
-        <v>894.3333333333334</v>
+        <v>975</v>
       </c>
       <c r="E28">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1191,13 +1191,13 @@
         <v>2</v>
       </c>
       <c r="C29">
-        <v>1024.545454545455</v>
+        <v>988</v>
       </c>
       <c r="D29">
         <v>1101</v>
       </c>
       <c r="E29">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1205,16 +1205,16 @@
         <v>32</v>
       </c>
       <c r="B30">
-        <v>1.928571428571429</v>
+        <v>2</v>
       </c>
       <c r="C30">
-        <v>644</v>
+        <v>645.3846153846154</v>
       </c>
       <c r="D30">
-        <v>1125</v>
+        <v>1075</v>
       </c>
       <c r="E30">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1222,13 +1222,13 @@
         <v>33</v>
       </c>
       <c r="B31">
-        <v>1.933333333333333</v>
+        <v>1.733333333333333</v>
       </c>
       <c r="C31">
-        <v>863.8235294117648</v>
+        <v>829.4117647058823</v>
       </c>
       <c r="D31">
-        <v>1063.166666666667</v>
+        <v>1006.4</v>
       </c>
       <c r="E31">
         <v>17</v>
@@ -1273,16 +1273,16 @@
         <v>36</v>
       </c>
       <c r="B34">
-        <v>2.282051282051282</v>
+        <v>2.317073170731707</v>
       </c>
       <c r="C34">
-        <v>826</v>
+        <v>824.8936170212766</v>
       </c>
       <c r="D34">
-        <v>1269.52380952381</v>
+        <v>1251.304347826087</v>
       </c>
       <c r="E34">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1290,16 +1290,16 @@
         <v>37</v>
       </c>
       <c r="B35">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="C35">
-        <v>851.5</v>
+        <v>820.625</v>
       </c>
       <c r="D35">
-        <v>1184.2</v>
+        <v>1025</v>
       </c>
       <c r="E35">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1321,16 +1321,16 @@
         <v>39</v>
       </c>
       <c r="B37">
-        <v>1.716417910447761</v>
+        <v>1.757142857142857</v>
       </c>
       <c r="C37">
-        <v>617.9736842105264</v>
+        <v>628.2625</v>
       </c>
       <c r="D37">
-        <v>814.12</v>
+        <v>824.6666666666666</v>
       </c>
       <c r="E37">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1338,16 +1338,16 @@
         <v>40</v>
       </c>
       <c r="B38">
-        <v>1.909090909090909</v>
+        <v>1.692307692307692</v>
       </c>
       <c r="C38">
-        <v>1245.357142857143</v>
+        <v>1275.625</v>
       </c>
       <c r="D38">
-        <v>1150</v>
+        <v>976.6666666666666</v>
       </c>
       <c r="E38">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1355,16 +1355,16 @@
         <v>41</v>
       </c>
       <c r="B39">
-        <v>2.111111111111111</v>
+        <v>2</v>
       </c>
       <c r="C39">
-        <v>1355.5</v>
+        <v>1302.727272727273</v>
       </c>
       <c r="D39">
         <v>1766.666666666667</v>
       </c>
       <c r="E39">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1389,16 +1389,16 @@
         <v>43</v>
       </c>
       <c r="B41">
-        <v>2.111111111111111</v>
+        <v>2.048780487804878</v>
       </c>
       <c r="C41">
-        <v>642.4137931034483</v>
+        <v>615.7142857142857</v>
       </c>
       <c r="D41">
-        <v>1211.5</v>
+        <v>1218.090909090909</v>
       </c>
       <c r="E41">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1406,16 +1406,16 @@
         <v>44</v>
       </c>
       <c r="B42">
-        <v>2.416666666666667</v>
+        <v>2.390243902439024</v>
       </c>
       <c r="C42">
-        <v>812.0857142857143</v>
+        <v>813.025</v>
       </c>
       <c r="D42">
-        <v>969.1428571428571</v>
+        <v>961.9411764705883</v>
       </c>
       <c r="E42">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1423,16 +1423,16 @@
         <v>45</v>
       </c>
       <c r="B43">
-        <v>1.896103896103896</v>
+        <v>1.9125</v>
       </c>
       <c r="C43">
-        <v>683.8101265822785</v>
+        <v>685.8915662650602</v>
       </c>
       <c r="D43">
-        <v>1034.666666666667</v>
+        <v>989.8709677419355</v>
       </c>
       <c r="E43">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1454,16 +1454,16 @@
         <v>47</v>
       </c>
       <c r="B45">
-        <v>1.909090909090909</v>
+        <v>1.846153846153846</v>
       </c>
       <c r="C45">
-        <v>733.5714285714286</v>
+        <v>729.6875</v>
       </c>
       <c r="D45">
-        <v>930</v>
+        <v>903.75</v>
       </c>
       <c r="E45">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1471,16 +1471,16 @@
         <v>48</v>
       </c>
       <c r="B46">
-        <v>2.090909090909091</v>
+        <v>2.3</v>
       </c>
       <c r="C46">
-        <v>3022.727272727273</v>
+        <v>3282.5</v>
       </c>
       <c r="D46">
-        <v>640</v>
+        <v>683.3333333333334</v>
       </c>
       <c r="E46">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1488,16 +1488,16 @@
         <v>49</v>
       </c>
       <c r="B47">
-        <v>2.009345794392523</v>
+        <v>1.981651376146789</v>
       </c>
       <c r="C47">
-        <v>1086.018518518518</v>
+        <v>1108.518181818182</v>
       </c>
       <c r="D47">
-        <v>1033.876543209876</v>
+        <v>1027.714285714286</v>
       </c>
       <c r="E47">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1525,13 +1525,13 @@
         <v>2.666666666666667</v>
       </c>
       <c r="C49">
-        <v>1281.428571428571</v>
+        <v>1411.666666666667</v>
       </c>
       <c r="D49">
         <v>1637.5</v>
       </c>
       <c r="E49">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1539,16 +1539,16 @@
         <v>52</v>
       </c>
       <c r="B50">
-        <v>2.107142857142857</v>
+        <v>2.103448275862069</v>
       </c>
       <c r="C50">
-        <v>807.4137931034483</v>
+        <v>806</v>
       </c>
       <c r="D50">
-        <v>1074.285714285714</v>
+        <v>1085.555555555556</v>
       </c>
       <c r="E50">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1556,16 +1556,16 @@
         <v>53</v>
       </c>
       <c r="B51">
-        <v>2.083333333333333</v>
+        <v>2.125</v>
       </c>
       <c r="C51">
-        <v>661.2</v>
+        <v>1032.164556962025</v>
       </c>
       <c r="D51">
-        <v>1085.5</v>
+        <v>1035.642857142857</v>
       </c>
       <c r="E51">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1573,16 +1573,16 @@
         <v>54</v>
       </c>
       <c r="B52">
-        <v>1.825</v>
+        <v>1.814814814814815</v>
       </c>
       <c r="C52">
-        <v>665.0864197530864</v>
+        <v>654.1084337349398</v>
       </c>
       <c r="D52">
-        <v>764.5599999999999</v>
+        <v>746.96</v>
       </c>
       <c r="E52">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1590,13 +1590,16 @@
         <v>55</v>
       </c>
       <c r="B53">
-        <v>3</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="C53">
-        <v>671.5</v>
+        <v>846</v>
+      </c>
+      <c r="D53">
+        <v>1406</v>
       </c>
       <c r="E53">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1604,16 +1607,16 @@
         <v>56</v>
       </c>
       <c r="B54">
-        <v>2.035714285714286</v>
+        <v>1.962962962962963</v>
       </c>
       <c r="C54">
-        <v>1131</v>
+        <v>1124.964285714286</v>
       </c>
       <c r="D54">
-        <v>1236.416666666667</v>
+        <v>1173.7</v>
       </c>
       <c r="E54">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1621,16 +1624,16 @@
         <v>57</v>
       </c>
       <c r="B55">
-        <v>2</v>
+        <v>2.03125</v>
       </c>
       <c r="C55">
-        <v>675.5405405405405</v>
+        <v>684.078947368421</v>
       </c>
       <c r="D55">
         <v>1100</v>
       </c>
       <c r="E55">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1638,13 +1641,13 @@
         <v>58</v>
       </c>
       <c r="B56">
-        <v>2.134146341463415</v>
+        <v>2.051020408163265</v>
       </c>
       <c r="C56">
-        <v>1036.183333333333</v>
+        <v>1205.083333333333</v>
       </c>
       <c r="D56">
-        <v>1257.172413793103</v>
+        <v>1306.054054054054</v>
       </c>
       <c r="E56">
         <v>120</v>
@@ -1655,13 +1658,13 @@
         <v>59</v>
       </c>
       <c r="B57">
-        <v>1.968421052631579</v>
+        <v>1.940594059405941</v>
       </c>
       <c r="C57">
-        <v>763.325</v>
+        <v>778.8833333333333</v>
       </c>
       <c r="D57">
-        <v>1047.125</v>
+        <v>1053.25</v>
       </c>
       <c r="E57">
         <v>120</v>
@@ -1672,13 +1675,13 @@
         <v>60</v>
       </c>
       <c r="B58">
-        <v>2.034782608695652</v>
+        <v>1.830508474576271</v>
       </c>
       <c r="C58">
-        <v>1519.75</v>
+        <v>1662.266666666667</v>
       </c>
       <c r="D58">
-        <v>1113.882352941177</v>
+        <v>1113.218181818182</v>
       </c>
       <c r="E58">
         <v>120</v>
@@ -1689,16 +1692,16 @@
         <v>61</v>
       </c>
       <c r="B59">
-        <v>2.375</v>
+        <v>2.383333333333333</v>
       </c>
       <c r="C59">
-        <v>803.1206896551724</v>
+        <v>791.7903225806451</v>
       </c>
       <c r="D59">
-        <v>1224.545454545455</v>
+        <v>1116.923076923077</v>
       </c>
       <c r="E59">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1706,13 +1709,13 @@
         <v>62</v>
       </c>
       <c r="B60">
-        <v>1.971698113207547</v>
+        <v>1.972222222222222</v>
       </c>
       <c r="C60">
-        <v>1253.705882352941</v>
+        <v>1275.294117647059</v>
       </c>
       <c r="D60">
-        <v>812.5</v>
+        <v>870.8333333333334</v>
       </c>
       <c r="E60">
         <v>120</v>
@@ -1723,13 +1726,13 @@
         <v>63</v>
       </c>
       <c r="B61">
-        <v>1.844036697247706</v>
+        <v>1.767241379310345</v>
       </c>
       <c r="C61">
-        <v>1174.076271186441</v>
+        <v>1137.216666666667</v>
       </c>
       <c r="D61">
-        <v>1016.125</v>
+        <v>1016.842105263158</v>
       </c>
       <c r="E61">
         <v>120</v>
@@ -1740,16 +1743,16 @@
         <v>64</v>
       </c>
       <c r="B62">
-        <v>2.347826086956522</v>
+        <v>2.421052631578947</v>
       </c>
       <c r="C62">
-        <v>887.8103448275862</v>
+        <v>889.3061224489796</v>
       </c>
       <c r="D62">
-        <v>1292.058823529412</v>
+        <v>1160.8125</v>
       </c>
       <c r="E62">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1757,13 +1760,13 @@
         <v>65</v>
       </c>
       <c r="B63">
-        <v>1.939655172413793</v>
+        <v>2.067226890756303</v>
       </c>
       <c r="C63">
-        <v>1090.741666666667</v>
+        <v>1155.775</v>
       </c>
       <c r="D63">
-        <v>1298.88679245283</v>
+        <v>1345.896551724138</v>
       </c>
       <c r="E63">
         <v>120</v>
@@ -1774,13 +1777,13 @@
         <v>66</v>
       </c>
       <c r="B64">
-        <v>1.752212389380531</v>
+        <v>1.787610619469026</v>
       </c>
       <c r="C64">
-        <v>846.5833333333334</v>
+        <v>848.0333333333333</v>
       </c>
       <c r="D64">
-        <v>750.2857142857143</v>
+        <v>752.7884615384615</v>
       </c>
       <c r="E64">
         <v>120</v>
@@ -1791,16 +1794,16 @@
         <v>67</v>
       </c>
       <c r="B65">
-        <v>2.456521739130435</v>
+        <v>2.523255813953488</v>
       </c>
       <c r="C65">
-        <v>914.5631067961165</v>
+        <v>907.6041666666666</v>
       </c>
       <c r="D65">
-        <v>1207.259259259259</v>
+        <v>1205.214285714286</v>
       </c>
       <c r="E65">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1808,13 +1811,13 @@
         <v>68</v>
       </c>
       <c r="B66">
-        <v>2.194444444444445</v>
+        <v>2.203703703703704</v>
       </c>
       <c r="C66">
-        <v>991.45</v>
+        <v>993.8083333333333</v>
       </c>
       <c r="D66">
-        <v>1258.943396226415</v>
+        <v>1274.833333333333</v>
       </c>
       <c r="E66">
         <v>120</v>
@@ -1825,13 +1828,13 @@
         <v>69</v>
       </c>
       <c r="B67">
-        <v>2.313725490196079</v>
+        <v>2.297029702970297</v>
       </c>
       <c r="C67">
-        <v>1012.966666666667</v>
+        <v>1030.226890756303</v>
       </c>
       <c r="D67">
-        <v>959.3493975903615</v>
+        <v>967</v>
       </c>
       <c r="E67">
         <v>120</v>
@@ -1842,13 +1845,13 @@
         <v>70</v>
       </c>
       <c r="B68">
-        <v>3.168316831683168</v>
+        <v>2.373626373626374</v>
       </c>
       <c r="C68">
-        <v>1805.666666666667</v>
+        <v>1613.358333333333</v>
       </c>
       <c r="D68">
-        <v>1058.727272727273</v>
+        <v>1271.25</v>
       </c>
       <c r="E68">
         <v>120</v>
@@ -1859,16 +1862,16 @@
         <v>71</v>
       </c>
       <c r="B69">
-        <v>2.485436893203883</v>
+        <v>2.531914893617021</v>
       </c>
       <c r="C69">
-        <v>1049.792452830189</v>
+        <v>1042.969072164949</v>
       </c>
       <c r="D69">
-        <v>1217.031578947368</v>
+        <v>1238.344827586207</v>
       </c>
       <c r="E69">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1876,16 +1879,16 @@
         <v>72</v>
       </c>
       <c r="B70">
-        <v>2.0625</v>
+        <v>2.052631578947369</v>
       </c>
       <c r="C70">
-        <v>1047.25</v>
+        <v>1051.649122807018</v>
       </c>
       <c r="D70">
-        <v>1206.826086956522</v>
+        <v>1264.277777777778</v>
       </c>
       <c r="E70">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -1893,13 +1896,13 @@
         <v>73</v>
       </c>
       <c r="B71">
-        <v>1.853211009174312</v>
+        <v>1.805555555555556</v>
       </c>
       <c r="C71">
-        <v>931.0252100840336</v>
+        <v>913.3193277310925</v>
       </c>
       <c r="D71">
-        <v>1208.259259259259</v>
+        <v>1166.48</v>
       </c>
       <c r="E71">
         <v>120</v>
@@ -1910,13 +1913,13 @@
         <v>74</v>
       </c>
       <c r="B72">
-        <v>1.766666666666667</v>
+        <v>1.636363636363636</v>
       </c>
       <c r="C72">
-        <v>1243.083333333333</v>
+        <v>1074.791666666667</v>
       </c>
       <c r="D72">
-        <v>952.9636363636364</v>
+        <v>957.265625</v>
       </c>
       <c r="E72">
         <v>120</v>
@@ -1927,13 +1930,13 @@
         <v>75</v>
       </c>
       <c r="B73">
-        <v>1.548672566371681</v>
+        <v>1.473684210526316</v>
       </c>
       <c r="C73">
-        <v>846.7666666666667</v>
+        <v>806.3666666666667</v>
       </c>
       <c r="D73">
-        <v>788.05</v>
+        <v>826.4625</v>
       </c>
       <c r="E73">
         <v>120</v>
@@ -1944,13 +1947,13 @@
         <v>76</v>
       </c>
       <c r="B74">
-        <v>1.833333333333333</v>
+        <v>1.80188679245283</v>
       </c>
       <c r="C74">
-        <v>1510.991666666667</v>
+        <v>1474.15</v>
       </c>
       <c r="D74">
-        <v>1168.397959183673</v>
+        <v>1001.959183673469</v>
       </c>
       <c r="E74">
         <v>120</v>
@@ -1961,16 +1964,16 @@
         <v>77</v>
       </c>
       <c r="B75">
-        <v>2.275862068965517</v>
+        <v>2.241379310344827</v>
       </c>
       <c r="C75">
-        <v>1105.466666666667</v>
+        <v>1073.40625</v>
       </c>
       <c r="D75">
-        <v>1348.411764705882</v>
+        <v>1345.722222222222</v>
       </c>
       <c r="E75">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1978,13 +1981,13 @@
         <v>78</v>
       </c>
       <c r="B76">
-        <v>1.821428571428571</v>
+        <v>1.848214285714286</v>
       </c>
       <c r="C76">
-        <v>970.9747899159664</v>
+        <v>1034.066666666667</v>
       </c>
       <c r="D76">
-        <v>1139.5</v>
+        <v>1196.845070422535</v>
       </c>
       <c r="E76">
         <v>120</v>
@@ -1995,13 +1998,13 @@
         <v>79</v>
       </c>
       <c r="B77">
-        <v>1.514285714285714</v>
+        <v>1.28695652173913</v>
       </c>
       <c r="C77">
-        <v>1416.641666666667</v>
+        <v>1492.441666666667</v>
       </c>
       <c r="D77">
-        <v>777.7843137254902</v>
+        <v>842.7831325301205</v>
       </c>
       <c r="E77">
         <v>120</v>
@@ -2012,16 +2015,16 @@
         <v>80</v>
       </c>
       <c r="B78">
-        <v>1.884615384615385</v>
+        <v>1.92</v>
       </c>
       <c r="C78">
-        <v>798</v>
+        <v>808.72</v>
       </c>
       <c r="D78">
-        <v>1124</v>
+        <v>1244</v>
       </c>
       <c r="E78">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -2029,13 +2032,13 @@
         <v>81</v>
       </c>
       <c r="B79">
-        <v>2.26605504587156</v>
+        <v>2.345132743362832</v>
       </c>
       <c r="C79">
-        <v>1524.725</v>
+        <v>1527.091666666667</v>
       </c>
       <c r="D79">
-        <v>975.0204081632653</v>
+        <v>974.3720930232558</v>
       </c>
       <c r="E79">
         <v>120</v>
@@ -2046,16 +2049,16 @@
         <v>82</v>
       </c>
       <c r="B80">
-        <v>2</v>
+        <v>1.909090909090909</v>
       </c>
       <c r="C80">
-        <v>876.6</v>
+        <v>856</v>
       </c>
       <c r="D80">
         <v>664.75</v>
       </c>
       <c r="E80">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -2063,13 +2066,13 @@
         <v>83</v>
       </c>
       <c r="B81">
-        <v>1.927272727272727</v>
+        <v>1.963636363636364</v>
       </c>
       <c r="C81">
-        <v>1275.739495798319</v>
+        <v>1278.655462184874</v>
       </c>
       <c r="D81">
-        <v>1452.272727272727</v>
+        <v>1443.181818181818</v>
       </c>
       <c r="E81">
         <v>120</v>
@@ -2080,16 +2083,16 @@
         <v>84</v>
       </c>
       <c r="B82">
-        <v>1.816901408450704</v>
+        <v>1.852941176470588</v>
       </c>
       <c r="C82">
-        <v>773.5</v>
+        <v>785.5</v>
       </c>
       <c r="D82">
-        <v>866.5555555555555</v>
+        <v>873.6666666666666</v>
       </c>
       <c r="E82">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -2097,16 +2100,16 @@
         <v>85</v>
       </c>
       <c r="B83">
-        <v>1.732758620689655</v>
+        <v>1.827272727272727</v>
       </c>
       <c r="C83">
-        <v>1037.308333333333</v>
+        <v>996.6521739130435</v>
       </c>
       <c r="D83">
-        <v>925.2916666666666</v>
+        <v>1025.911764705882</v>
       </c>
       <c r="E83">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -2114,16 +2117,16 @@
         <v>86</v>
       </c>
       <c r="B84">
-        <v>1.566666666666667</v>
+        <v>1.590163934426229</v>
       </c>
       <c r="C84">
-        <v>1062.515625</v>
+        <v>1061.938461538462</v>
       </c>
       <c r="D84">
-        <v>1303.923076923077</v>
+        <v>1282.214285714286</v>
       </c>
       <c r="E84">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -2131,13 +2134,13 @@
         <v>87</v>
       </c>
       <c r="B85">
-        <v>1.693693693693694</v>
+        <v>1.536363636363636</v>
       </c>
       <c r="C85">
-        <v>1405.116666666667</v>
+        <v>1359.633333333333</v>
       </c>
       <c r="D85">
-        <v>917.4222222222222</v>
+        <v>969.7021276595744</v>
       </c>
       <c r="E85">
         <v>120</v>
@@ -2148,16 +2151,16 @@
         <v>88</v>
       </c>
       <c r="B86">
-        <v>1.717391304347826</v>
+        <v>1.717171717171717</v>
       </c>
       <c r="C86">
-        <v>872.5436893203884</v>
+        <v>850.8660714285714</v>
       </c>
       <c r="D86">
-        <v>1187.694444444444</v>
+        <v>1231.878787878788</v>
       </c>
       <c r="E86">
-        <v>103</v>
+        <v>112</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -2165,16 +2168,16 @@
         <v>89</v>
       </c>
       <c r="B87">
-        <v>2.050632911392405</v>
+        <v>1.976744186046512</v>
       </c>
       <c r="C87">
-        <v>877.3820224719101</v>
+        <v>856.1354166666666</v>
       </c>
       <c r="D87">
-        <v>1189.166666666667</v>
+        <v>1036.333333333333</v>
       </c>
       <c r="E87">
-        <v>89</v>
+        <v>96</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -2182,16 +2185,16 @@
         <v>90</v>
       </c>
       <c r="B88">
-        <v>2.018867924528302</v>
+        <v>2.017241379310345</v>
       </c>
       <c r="C88">
-        <v>779.6896551724138</v>
+        <v>779.9047619047619</v>
       </c>
       <c r="D88">
-        <v>962.3571428571429</v>
+        <v>933.6470588235294</v>
       </c>
       <c r="E88">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -2199,16 +2202,16 @@
         <v>91</v>
       </c>
       <c r="B89">
-        <v>1.795454545454545</v>
+        <v>2.060606060606061</v>
       </c>
       <c r="C89">
-        <v>872.0862068965517</v>
+        <v>950.5106382978723</v>
       </c>
       <c r="D89">
-        <v>1049.625</v>
+        <v>1085.727272727273</v>
       </c>
       <c r="E89">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -2216,13 +2219,13 @@
         <v>92</v>
       </c>
       <c r="B90">
-        <v>1.482758620689655</v>
+        <v>1.594827586206897</v>
       </c>
       <c r="C90">
-        <v>3124.116666666667</v>
+        <v>980.2083333333334</v>
       </c>
       <c r="D90">
-        <v>887.7564102564103</v>
+        <v>871.9111111111112</v>
       </c>
       <c r="E90">
         <v>120</v>
@@ -2233,16 +2236,16 @@
         <v>93</v>
       </c>
       <c r="B91">
-        <v>3.240740740740741</v>
+        <v>3.298245614035088</v>
       </c>
       <c r="C91">
-        <v>2227.363636363636</v>
+        <v>2285.948275862069</v>
       </c>
       <c r="D91">
-        <v>1910</v>
+        <v>1820.555555555556</v>
       </c>
       <c r="E91">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -2250,16 +2253,16 @@
         <v>94</v>
       </c>
       <c r="B92">
-        <v>2.333333333333333</v>
+        <v>2.4</v>
       </c>
       <c r="C92">
-        <v>878.2777777777778</v>
+        <v>829.7619047619048</v>
       </c>
       <c r="D92">
         <v>1870</v>
       </c>
       <c r="E92">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -2267,13 +2270,13 @@
         <v>95</v>
       </c>
       <c r="B93">
-        <v>1.391666666666667</v>
+        <v>1.408333333333333</v>
       </c>
       <c r="C93">
-        <v>1226.083333333333</v>
+        <v>1198.75</v>
       </c>
       <c r="D93">
-        <v>839.2222222222222</v>
+        <v>835.771186440678</v>
       </c>
       <c r="E93">
         <v>120</v>
@@ -2284,16 +2287,16 @@
         <v>96</v>
       </c>
       <c r="B94">
-        <v>2.133333333333333</v>
+        <v>2.411764705882353</v>
       </c>
       <c r="C94">
-        <v>1273.611111111111</v>
+        <v>1386.764705882353</v>
       </c>
       <c r="D94">
-        <v>1840.333333333333</v>
+        <v>1805.727272727273</v>
       </c>
       <c r="E94">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -2301,13 +2304,13 @@
         <v>97</v>
       </c>
       <c r="B95">
-        <v>3.130434782608696</v>
+        <v>3.160714285714286</v>
       </c>
       <c r="C95">
-        <v>1783.941666666667</v>
+        <v>1832.35</v>
       </c>
       <c r="D95">
-        <v>2449.125</v>
+        <v>2457.222222222222</v>
       </c>
       <c r="E95">
         <v>120</v>
@@ -2397,16 +2400,16 @@
         <v>103</v>
       </c>
       <c r="B101">
-        <v>2.16</v>
+        <v>2.038461538461538</v>
       </c>
       <c r="C101">
-        <v>1276.551724137931</v>
+        <v>1286.166666666667</v>
       </c>
       <c r="D101">
-        <v>1250.333333333333</v>
+        <v>1165.285714285714</v>
       </c>
       <c r="E101">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -2414,16 +2417,16 @@
         <v>104</v>
       </c>
       <c r="B102">
-        <v>1.265625</v>
+        <v>1.25</v>
       </c>
       <c r="C102">
-        <v>749.1076923076923</v>
+        <v>748.5507246376811</v>
       </c>
       <c r="D102">
-        <v>800.4615384615385</v>
+        <v>776.0666666666667</v>
       </c>
       <c r="E102">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -2454,7 +2457,7 @@
         <v>1200</v>
       </c>
       <c r="E104">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -2462,16 +2465,16 @@
         <v>107</v>
       </c>
       <c r="B105">
-        <v>1.952380952380952</v>
+        <v>2</v>
       </c>
       <c r="C105">
-        <v>682</v>
+        <v>706.7692307692307</v>
       </c>
       <c r="D105">
         <v>855</v>
       </c>
       <c r="E105">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2479,16 +2482,16 @@
         <v>108</v>
       </c>
       <c r="B106">
-        <v>2.333333333333333</v>
+        <v>2.4</v>
       </c>
       <c r="C106">
-        <v>730.5555555555555</v>
+        <v>732.5</v>
       </c>
       <c r="D106">
         <v>1200</v>
       </c>
       <c r="E106">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -2496,30 +2499,33 @@
         <v>109</v>
       </c>
       <c r="B107">
-        <v>2</v>
+        <v>1.785714285714286</v>
       </c>
       <c r="C107">
-        <v>785.3571428571429</v>
+        <v>768.125</v>
       </c>
       <c r="D107">
-        <v>1052</v>
+        <v>950</v>
       </c>
       <c r="E107">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="B108">
+        <v>3</v>
+      </c>
       <c r="C108">
-        <v>635</v>
+        <v>1242.5</v>
       </c>
       <c r="D108">
-        <v>780</v>
+        <v>1564</v>
       </c>
       <c r="E108">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -2527,16 +2533,16 @@
         <v>111</v>
       </c>
       <c r="B109">
-        <v>1.829268292682927</v>
+        <v>1.86046511627907</v>
       </c>
       <c r="C109">
-        <v>797.9047619047619</v>
+        <v>794.8139534883721</v>
       </c>
       <c r="D109">
-        <v>950.25</v>
+        <v>1029.153846153846</v>
       </c>
       <c r="E109">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -2544,16 +2550,16 @@
         <v>112</v>
       </c>
       <c r="B110">
-        <v>1.621621621621622</v>
+        <v>1.560975609756098</v>
       </c>
       <c r="C110">
-        <v>1565.263157894737</v>
+        <v>1568.095238095238</v>
       </c>
       <c r="D110">
-        <v>978.516129032258</v>
+        <v>973.8857142857142</v>
       </c>
       <c r="E110">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -2561,16 +2567,16 @@
         <v>113</v>
       </c>
       <c r="B111">
-        <v>2.1875</v>
+        <v>2.3</v>
       </c>
       <c r="C111">
-        <v>733.1764705882352</v>
+        <v>752.5833333333334</v>
       </c>
       <c r="D111">
         <v>900</v>
       </c>
       <c r="E111">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -2578,16 +2584,16 @@
         <v>114</v>
       </c>
       <c r="B112">
-        <v>2.217391304347826</v>
+        <v>2.275</v>
       </c>
       <c r="C112">
-        <v>781.7254901960785</v>
+        <v>786.1111111111111</v>
       </c>
       <c r="D112">
-        <v>992.1904761904761</v>
+        <v>994.8421052631579</v>
       </c>
       <c r="E112">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -2595,16 +2601,16 @@
         <v>115</v>
       </c>
       <c r="B113">
-        <v>2.333333333333333</v>
+        <v>2.25</v>
       </c>
       <c r="C113">
-        <v>575</v>
+        <v>522.5</v>
       </c>
       <c r="D113">
         <v>1700</v>
       </c>
       <c r="E113">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -2612,16 +2618,16 @@
         <v>116</v>
       </c>
       <c r="B114">
-        <v>1.925925925925926</v>
+        <v>1.796875</v>
       </c>
       <c r="C114">
-        <v>1643.070175438596</v>
+        <v>1633.731343283582</v>
       </c>
       <c r="D114">
-        <v>1102.068181818182</v>
+        <v>1079.5</v>
       </c>
       <c r="E114">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -2629,16 +2635,16 @@
         <v>117</v>
       </c>
       <c r="B115">
-        <v>2.222222222222222</v>
+        <v>2.25</v>
       </c>
       <c r="C115">
-        <v>751.8181818181819</v>
+        <v>765.7142857142857</v>
       </c>
       <c r="D115">
-        <v>933.3333333333334</v>
+        <v>1040</v>
       </c>
       <c r="E115">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>